<commit_message>
alittle cleanup on the transform
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-VA.MHV.PHR.LabSpecimen.xlsx
+++ b/docs/StructureDefinition-VA.MHV.PHR.LabSpecimen.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.3-beta</t>
+    <t>0.1.4-beta</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-02-02T16:50:30-06:00</t>
+    <t>2023-02-03T09:54:41-06:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
add full set of examples as transformed by xslt
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-VA.MHV.PHR.LabSpecimen.xlsx
+++ b/docs/StructureDefinition-VA.MHV.PHR.LabSpecimen.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.4-beta</t>
+    <t>0.1.5-beta</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-02-21T15:24:44-06:00</t>
+    <t>2023-02-23T08:24:10-06:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
add BP and Pain distinction
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-VA.MHV.PHR.LabSpecimen.xlsx
+++ b/docs/StructureDefinition-VA.MHV.PHR.LabSpecimen.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2290" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2290" uniqueCount="446">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-03-29T16:54:48-05:00</t>
+    <t>2023-03-30T12:22:18-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -645,6 +645,10 @@
   </si>
   <si>
     <t>Identifier.system</t>
+  </si>
+  <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+TOid-startswithoid:ID system must start with urn:oid:2.16.840.1.113883.4.349.4. The next would be the {stationNbr} {value.startsWith('urn:oid:2.16.840.1.113883.4.349.4.')}</t>
   </si>
   <si>
     <t>II.root or Role.id.root</t>
@@ -3690,16 +3694,16 @@
         <v>77</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>98</v>
+        <v>200</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="AL17" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AM17" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="AN17" t="s" s="2">
         <v>77</v>
@@ -3707,10 +3711,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s" s="2">
@@ -3736,13 +3740,13 @@
         <v>157</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="N18" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="O18" s="2"/>
       <c r="P18" t="s" s="2">
@@ -3756,7 +3760,7 @@
         <v>77</v>
       </c>
       <c r="T18" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="U18" t="s" s="2">
         <v>77</v>
@@ -3792,7 +3796,7 @@
         <v>77</v>
       </c>
       <c r="AF18" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="AG18" t="s" s="2">
         <v>78</v>
@@ -3807,13 +3811,13 @@
         <v>98</v>
       </c>
       <c r="AK18" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="AL18" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="AN18" t="s" s="2">
         <v>77</v>
@@ -3821,10 +3825,10 @@
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s" s="2">
@@ -3847,13 +3851,13 @@
         <v>87</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
@@ -3904,7 +3908,7 @@
         <v>77</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="AG19" t="s" s="2">
         <v>78</v>
@@ -3919,13 +3923,13 @@
         <v>98</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="AL19" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="AN19" t="s" s="2">
         <v>77</v>
@@ -3933,10 +3937,10 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s" s="2">
@@ -3959,16 +3963,16 @@
         <v>87</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="N20" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="O20" s="2"/>
       <c r="P20" t="s" s="2">
@@ -4018,7 +4022,7 @@
         <v>77</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="AG20" t="s" s="2">
         <v>78</v>
@@ -4033,13 +4037,13 @@
         <v>98</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="AL20" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="AN20" t="s" s="2">
         <v>77</v>
@@ -4047,10 +4051,10 @@
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s" s="2">
@@ -4076,10 +4080,10 @@
         <v>144</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
@@ -4130,7 +4134,7 @@
         <v>77</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>78</v>
@@ -4145,24 +4149,24 @@
         <v>98</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="AL21" t="s" s="2">
         <v>150</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="AN21" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
@@ -4188,13 +4192,13 @@
         <v>106</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="N22" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="O22" s="2"/>
       <c r="P22" t="s" s="2">
@@ -4223,10 +4227,10 @@
         <v>175</v>
       </c>
       <c r="Y22" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="Z22" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="AA22" t="s" s="2">
         <v>77</v>
@@ -4244,7 +4248,7 @@
         <v>77</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>78</v>
@@ -4259,24 +4263,24 @@
         <v>98</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="AN22" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
@@ -4302,13 +4306,13 @@
         <v>182</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="N23" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="O23" s="2"/>
       <c r="P23" t="s" s="2">
@@ -4334,13 +4338,13 @@
         <v>77</v>
       </c>
       <c r="X23" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="Y23" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="Z23" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AA23" t="s" s="2">
         <v>77</v>
@@ -4358,7 +4362,7 @@
         <v>77</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>78</v>
@@ -4373,13 +4377,13 @@
         <v>98</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN23" t="s" s="2">
         <v>77</v>
@@ -4387,10 +4391,10 @@
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
@@ -4499,10 +4503,10 @@
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
@@ -4613,10 +4617,10 @@
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
@@ -4639,19 +4643,19 @@
         <v>87</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="N26" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="O26" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="P26" t="s" s="2">
         <v>77</v>
@@ -4700,7 +4704,7 @@
         <v>77</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>78</v>
@@ -4715,13 +4719,13 @@
         <v>98</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AL26" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN26" t="s" s="2">
         <v>77</v>
@@ -4729,10 +4733,10 @@
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
@@ -4758,16 +4762,16 @@
         <v>157</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="N27" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="O27" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="P27" t="s" s="2">
         <v>77</v>
@@ -4816,7 +4820,7 @@
         <v>77</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>78</v>
@@ -4831,24 +4835,24 @@
         <v>98</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="AL27" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="AN27" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
@@ -4871,17 +4875,17 @@
         <v>87</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="P28" t="s" s="2">
         <v>77</v>
@@ -4930,7 +4934,7 @@
         <v>77</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>78</v>
@@ -4945,24 +4949,24 @@
         <v>98</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="AM28" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AN28" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
@@ -4985,13 +4989,13 @@
         <v>87</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
@@ -5042,7 +5046,7 @@
         <v>77</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>78</v>
@@ -5057,13 +5061,13 @@
         <v>98</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="AN29" t="s" s="2">
         <v>77</v>
@@ -5071,10 +5075,10 @@
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -5097,16 +5101,16 @@
         <v>77</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="N30" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="O30" s="2"/>
       <c r="P30" t="s" s="2">
@@ -5156,7 +5160,7 @@
         <v>77</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>78</v>
@@ -5171,7 +5175,7 @@
         <v>98</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="AL30" t="s" s="2">
         <v>77</v>
@@ -5185,10 +5189,10 @@
     </row>
     <row r="31">
       <c r="A31" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -5211,16 +5215,16 @@
         <v>77</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="N31" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="O31" s="2"/>
       <c r="P31" t="s" s="2">
@@ -5270,7 +5274,7 @@
         <v>77</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>78</v>
@@ -5285,13 +5289,13 @@
         <v>98</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>77</v>
@@ -5299,10 +5303,10 @@
     </row>
     <row r="32">
       <c r="A32" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -5325,13 +5329,13 @@
         <v>77</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
@@ -5382,7 +5386,7 @@
         <v>77</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>78</v>
@@ -5397,13 +5401,13 @@
         <v>98</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="AL32" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>77</v>
@@ -5411,10 +5415,10 @@
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -5523,10 +5527,10 @@
     </row>
     <row r="34">
       <c r="A34" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -5637,14 +5641,14 @@
     </row>
     <row r="35">
       <c r="A35" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" t="s" s="2">
@@ -5666,10 +5670,10 @@
         <v>132</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="N35" t="s" s="2">
         <v>135</v>
@@ -5724,7 +5728,7 @@
         <v>77</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>78</v>
@@ -5753,10 +5757,10 @@
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -5779,13 +5783,13 @@
         <v>87</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
@@ -5836,7 +5840,7 @@
         <v>77</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>78</v>
@@ -5851,13 +5855,13 @@
         <v>98</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="AN36" t="s" s="2">
         <v>77</v>
@@ -5865,10 +5869,10 @@
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -5891,13 +5895,13 @@
         <v>87</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
@@ -5936,7 +5940,7 @@
         <v>77</v>
       </c>
       <c r="AB37" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="AC37" s="2"/>
       <c r="AD37" t="s" s="2">
@@ -5946,7 +5950,7 @@
         <v>148</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>78</v>
@@ -5961,13 +5965,13 @@
         <v>98</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>77</v>
@@ -5975,13 +5979,13 @@
     </row>
     <row r="38">
       <c r="A38" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C38" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D38" t="s" s="2">
         <v>77</v>
@@ -6003,13 +6007,13 @@
         <v>87</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
@@ -6060,7 +6064,7 @@
         <v>77</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>78</v>
@@ -6075,24 +6079,24 @@
         <v>98</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="AN38" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
@@ -6115,13 +6119,13 @@
         <v>87</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
@@ -6172,7 +6176,7 @@
         <v>77</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>78</v>
@@ -6190,7 +6194,7 @@
         <v>77</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AM39" t="s" s="2">
         <v>77</v>
@@ -6201,10 +6205,10 @@
     </row>
     <row r="40">
       <c r="A40" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -6227,13 +6231,13 @@
         <v>77</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
@@ -6284,7 +6288,7 @@
         <v>77</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>78</v>
@@ -6299,13 +6303,13 @@
         <v>98</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="AL40" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>77</v>
@@ -6313,10 +6317,10 @@
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -6342,10 +6346,10 @@
         <v>182</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
@@ -6372,13 +6376,13 @@
         <v>77</v>
       </c>
       <c r="X41" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="Y41" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="Z41" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="AA41" t="s" s="2">
         <v>77</v>
@@ -6396,7 +6400,7 @@
         <v>77</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>78</v>
@@ -6411,13 +6415,13 @@
         <v>98</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="AL41" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>77</v>
@@ -6425,10 +6429,10 @@
     </row>
     <row r="42">
       <c r="A42" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -6454,13 +6458,13 @@
         <v>182</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="N42" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="O42" s="2"/>
       <c r="P42" t="s" s="2">
@@ -6486,13 +6490,13 @@
         <v>77</v>
       </c>
       <c r="X42" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="Y42" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="Z42" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="AA42" t="s" s="2">
         <v>77</v>
@@ -6510,7 +6514,7 @@
         <v>77</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>78</v>
@@ -6525,13 +6529,13 @@
         <v>98</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="AL42" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>77</v>
@@ -6539,10 +6543,10 @@
     </row>
     <row r="43">
       <c r="A43" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -6565,19 +6569,19 @@
         <v>87</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="N43" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="O43" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="P43" t="s" s="2">
         <v>77</v>
@@ -6605,10 +6609,10 @@
         <v>187</v>
       </c>
       <c r="Y43" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="Z43" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AA43" t="s" s="2">
         <v>77</v>
@@ -6626,7 +6630,7 @@
         <v>77</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>78</v>
@@ -6647,7 +6651,7 @@
         <v>77</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>77</v>
@@ -6655,10 +6659,10 @@
     </row>
     <row r="44">
       <c r="A44" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -6681,13 +6685,13 @@
         <v>77</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
@@ -6738,7 +6742,7 @@
         <v>77</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>78</v>
@@ -6753,7 +6757,7 @@
         <v>98</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="AL44" t="s" s="2">
         <v>77</v>
@@ -6767,10 +6771,10 @@
     </row>
     <row r="45">
       <c r="A45" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -6879,10 +6883,10 @@
     </row>
     <row r="46">
       <c r="A46" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
@@ -6993,14 +6997,14 @@
     </row>
     <row r="47">
       <c r="A47" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" t="s" s="2">
@@ -7022,10 +7026,10 @@
         <v>132</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="N47" t="s" s="2">
         <v>135</v>
@@ -7080,7 +7084,7 @@
         <v>77</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>78</v>
@@ -7109,10 +7113,10 @@
     </row>
     <row r="48">
       <c r="A48" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -7138,10 +7142,10 @@
         <v>157</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="N48" s="2"/>
       <c r="O48" s="2"/>
@@ -7192,7 +7196,7 @@
         <v>77</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>78</v>
@@ -7207,7 +7211,7 @@
         <v>98</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="AL48" t="s" s="2">
         <v>77</v>
@@ -7221,10 +7225,10 @@
     </row>
     <row r="49">
       <c r="A49" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
@@ -7250,10 +7254,10 @@
         <v>182</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" s="2"/>
@@ -7280,13 +7284,13 @@
         <v>77</v>
       </c>
       <c r="X49" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="Y49" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="Z49" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="AA49" t="s" s="2">
         <v>77</v>
@@ -7304,7 +7308,7 @@
         <v>77</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>78</v>
@@ -7319,7 +7323,7 @@
         <v>98</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AL49" t="s" s="2">
         <v>77</v>
@@ -7333,10 +7337,10 @@
     </row>
     <row r="50">
       <c r="A50" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
@@ -7359,13 +7363,13 @@
         <v>77</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="N50" s="2"/>
       <c r="O50" s="2"/>
@@ -7416,7 +7420,7 @@
         <v>77</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>78</v>
@@ -7431,13 +7435,13 @@
         <v>98</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="AL50" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="AN50" t="s" s="2">
         <v>77</v>
@@ -7445,10 +7449,10 @@
     </row>
     <row r="51">
       <c r="A51" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
@@ -7471,13 +7475,13 @@
         <v>77</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
@@ -7528,7 +7532,7 @@
         <v>77</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>78</v>
@@ -7543,7 +7547,7 @@
         <v>98</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="AL51" t="s" s="2">
         <v>77</v>
@@ -7557,10 +7561,10 @@
     </row>
     <row r="52">
       <c r="A52" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
@@ -7583,13 +7587,13 @@
         <v>77</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="N52" s="2"/>
       <c r="O52" s="2"/>
@@ -7640,7 +7644,7 @@
         <v>77</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>78</v>
@@ -7655,7 +7659,7 @@
         <v>98</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="AL52" t="s" s="2">
         <v>77</v>
@@ -7669,10 +7673,10 @@
     </row>
     <row r="53">
       <c r="A53" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
@@ -7781,10 +7785,10 @@
     </row>
     <row r="54">
       <c r="A54" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" t="s" s="2">
@@ -7895,14 +7899,14 @@
     </row>
     <row r="55">
       <c r="A55" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" t="s" s="2">
@@ -7924,10 +7928,10 @@
         <v>132</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="N55" t="s" s="2">
         <v>135</v>
@@ -7982,7 +7986,7 @@
         <v>77</v>
       </c>
       <c r="AF55" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="AG55" t="s" s="2">
         <v>78</v>
@@ -8011,10 +8015,10 @@
     </row>
     <row r="56">
       <c r="A56" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" t="s" s="2">
@@ -8040,10 +8044,10 @@
         <v>144</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="N56" s="2"/>
       <c r="O56" s="2"/>
@@ -8094,7 +8098,7 @@
         <v>77</v>
       </c>
       <c r="AF56" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="AG56" t="s" s="2">
         <v>78</v>
@@ -8115,7 +8119,7 @@
         <v>77</v>
       </c>
       <c r="AM56" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="AN56" t="s" s="2">
         <v>77</v>
@@ -8123,10 +8127,10 @@
     </row>
     <row r="57">
       <c r="A57" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" t="s" s="2">
@@ -8152,10 +8156,10 @@
         <v>157</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="N57" s="2"/>
       <c r="O57" s="2"/>
@@ -8206,7 +8210,7 @@
         <v>77</v>
       </c>
       <c r="AF57" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="AG57" t="s" s="2">
         <v>78</v>
@@ -8221,7 +8225,7 @@
         <v>98</v>
       </c>
       <c r="AK57" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="AL57" t="s" s="2">
         <v>77</v>
@@ -8235,10 +8239,10 @@
     </row>
     <row r="58">
       <c r="A58" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" t="s" s="2">
@@ -8264,10 +8268,10 @@
         <v>182</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="N58" s="2"/>
       <c r="O58" s="2"/>
@@ -8294,13 +8298,13 @@
         <v>77</v>
       </c>
       <c r="X58" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="Y58" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="Z58" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="AA58" t="s" s="2">
         <v>77</v>
@@ -8318,7 +8322,7 @@
         <v>77</v>
       </c>
       <c r="AF58" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="AG58" t="s" s="2">
         <v>78</v>
@@ -8333,13 +8337,13 @@
         <v>98</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AL58" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AM58" t="s" s="2">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="AN58" t="s" s="2">
         <v>77</v>
@@ -8347,10 +8351,10 @@
     </row>
     <row r="59">
       <c r="A59" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s" s="2">
@@ -8373,13 +8377,13 @@
         <v>77</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="N59" s="2"/>
       <c r="O59" s="2"/>
@@ -8430,7 +8434,7 @@
         <v>77</v>
       </c>
       <c r="AF59" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="AG59" t="s" s="2">
         <v>78</v>
@@ -8445,13 +8449,13 @@
         <v>98</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="AL59" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AM59" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="AN59" t="s" s="2">
         <v>77</v>
@@ -8459,10 +8463,10 @@
     </row>
     <row r="60">
       <c r="A60" t="s" s="2">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" t="s" s="2">
@@ -8485,13 +8489,13 @@
         <v>77</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="N60" s="2"/>
       <c r="O60" s="2"/>
@@ -8542,7 +8546,7 @@
         <v>77</v>
       </c>
       <c r="AF60" t="s" s="2">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="AG60" t="s" s="2">
         <v>78</v>
@@ -8557,13 +8561,13 @@
         <v>98</v>
       </c>
       <c r="AK60" t="s" s="2">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="AL60" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AM60" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AN60" t="s" s="2">
         <v>77</v>
@@ -8571,10 +8575,10 @@
     </row>
     <row r="61">
       <c r="A61" t="s" s="2">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B61" t="s" s="2">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" t="s" s="2">
@@ -8597,13 +8601,13 @@
         <v>77</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="N61" s="2"/>
       <c r="O61" s="2"/>
@@ -8630,13 +8634,13 @@
         <v>77</v>
       </c>
       <c r="X61" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="Y61" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="Z61" t="s" s="2">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="AA61" t="s" s="2">
         <v>77</v>
@@ -8654,7 +8658,7 @@
         <v>77</v>
       </c>
       <c r="AF61" t="s" s="2">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="AG61" t="s" s="2">
         <v>78</v>
@@ -8669,13 +8673,13 @@
         <v>98</v>
       </c>
       <c r="AK61" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="AL61" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AM61" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="AN61" t="s" s="2">
         <v>77</v>
@@ -8683,10 +8687,10 @@
     </row>
     <row r="62">
       <c r="A62" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" t="s" s="2">
@@ -8712,16 +8716,16 @@
         <v>182</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="M62" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="N62" t="s" s="2">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="O62" t="s" s="2">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="P62" t="s" s="2">
         <v>77</v>
@@ -8749,10 +8753,10 @@
         <v>187</v>
       </c>
       <c r="Y62" t="s" s="2">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="Z62" t="s" s="2">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="AA62" t="s" s="2">
         <v>77</v>
@@ -8770,7 +8774,7 @@
         <v>77</v>
       </c>
       <c r="AF62" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="AG62" t="s" s="2">
         <v>78</v>
@@ -8791,7 +8795,7 @@
         <v>77</v>
       </c>
       <c r="AM62" t="s" s="2">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="AN62" t="s" s="2">
         <v>77</v>
@@ -8799,10 +8803,10 @@
     </row>
     <row r="63">
       <c r="A63" t="s" s="2">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B63" t="s" s="2">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" t="s" s="2">
@@ -8825,13 +8829,13 @@
         <v>77</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="L63" t="s" s="2">
         <v>50</v>
       </c>
       <c r="M63" t="s" s="2">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="N63" s="2"/>
       <c r="O63" s="2"/>
@@ -8882,7 +8886,7 @@
         <v>77</v>
       </c>
       <c r="AF63" t="s" s="2">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="AG63" t="s" s="2">
         <v>78</v>
@@ -8897,13 +8901,13 @@
         <v>98</v>
       </c>
       <c r="AK63" t="s" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="AL63" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AM63" t="s" s="2">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="AN63" t="s" s="2">
         <v>77</v>

</xml_diff>

<commit_message>
finish vitals and chem-hem mapping
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-VA.MHV.PHR.LabSpecimen.xlsx
+++ b/docs/StructureDefinition-VA.MHV.PHR.LabSpecimen.xlsx
@@ -9,11 +9,14 @@
     <sheet name="Metadata" r:id="rId3" sheetId="1"/>
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AN$63</definedName>
+  </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2290" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2290" uniqueCount="445">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-03-31T07:50:38-05:00</t>
+    <t>2023-04-11T08:45:33-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -81,16 +84,15 @@
     <t>Description</t>
   </si>
   <si>
-    <t>A profile showing how the LabSpecimenTO is mapped into a FHIR Specimen.
-- This is usually a contained resource, contained in the Lab Report or the Lab Test. The use of contained is for simplicity sake and to limit the need to manage Specimen resource instances
+    <t>A profile showing how the `LabSpecimenTO` is mapped into a FHIR Specimen.
+- This is a contained resource, contained in the Lab Report or the Lab Test. The use of contained is for simplicity sake and to limit the need to manage Specimen resource instances
 - must have a type 
-  - Specimen.type.text &lt;- LabSpecimenTO.name
+  - `Specimen.type.text` &lt;- `LabSpecimenTO.name`
   - type should be a code derived from LabSpecimenTO.name
-- should have a collectedDateTime derived from LabSpecimenTO.collectionDate
-- may have an identifier - Specimen.identifier &lt;- LabSpecimenTO.id
-  - if no LabSpecimenTO.id is given, then the Specimen resource must be contained
-- should have an accessionIdentifier derived from LabSpecimenTO.accessionNum
-- should have a subject (unless Contained)
+- should have a `collectedDateTime` derived from `LabSpecimenTO.collectionDate`
+- may have an `identifier` - `Specimen.identifier` &lt;- `LabSpecimenTO.id`
+  - if no `LabSpecimenTO.id` is given, then the Specimen resource must be contained
+- should have an `accessionIdentifier` derived from `LabSpecimenTO.accessionNum`
 TODO questions: 
 - examples didn't have much populated
 - not clear what site and facility might contain, so can't tell where they would go
@@ -896,9 +898,6 @@
   </si>
   <si>
     <t>FiveWs.subject</t>
-  </si>
-  <si>
-    <t>patient</t>
   </si>
   <si>
     <t>Specimen.receivedTime</t>
@@ -1531,6 +1530,21 @@
       <alignment vertical="top" wrapText="true"/>
     </xf>
   </cellXfs>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="22"/>
+        <i val="true"/>
+      </font>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -1887,7 +1901,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" hidden="true">
       <c r="A2" t="s" s="2">
         <v>30</v>
       </c>
@@ -1999,7 +2013,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" hidden="true">
       <c r="A3" t="s" s="2">
         <v>85</v>
       </c>
@@ -2113,7 +2127,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" hidden="true">
       <c r="A4" t="s" s="2">
         <v>93</v>
       </c>
@@ -2225,7 +2239,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
         <v>99</v>
       </c>
@@ -2339,7 +2353,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
         <v>105</v>
       </c>
@@ -2453,7 +2467,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" hidden="true">
       <c r="A7" t="s" s="2">
         <v>114</v>
       </c>
@@ -2567,7 +2581,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
         <v>122</v>
       </c>
@@ -2681,7 +2695,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
         <v>130</v>
       </c>
@@ -2795,7 +2809,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
         <v>138</v>
       </c>
@@ -2911,7 +2925,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
         <v>143</v>
       </c>
@@ -3021,7 +3035,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
         <v>153</v>
       </c>
@@ -3135,7 +3149,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
         <v>155</v>
       </c>
@@ -3247,7 +3261,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
         <v>162</v>
       </c>
@@ -3361,7 +3375,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
         <v>168</v>
       </c>
@@ -3477,7 +3491,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
         <v>180</v>
       </c>
@@ -3593,7 +3607,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
         <v>192</v>
       </c>
@@ -3709,7 +3723,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
         <v>203</v>
       </c>
@@ -3823,7 +3837,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
         <v>212</v>
       </c>
@@ -3935,7 +3949,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
         <v>220</v>
       </c>
@@ -4049,7 +4063,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
         <v>229</v>
       </c>
@@ -4161,7 +4175,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
         <v>235</v>
       </c>
@@ -4275,7 +4289,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
         <v>245</v>
       </c>
@@ -4288,13 +4302,13 @@
       </c>
       <c r="E23" s="2"/>
       <c r="F23" t="s" s="2">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="G23" t="s" s="2">
         <v>86</v>
       </c>
       <c r="H23" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="I23" t="s" s="2">
         <v>77</v>
@@ -4389,7 +4403,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
         <v>255</v>
       </c>
@@ -4501,7 +4515,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
         <v>256</v>
       </c>
@@ -4615,7 +4629,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
         <v>257</v>
       </c>
@@ -4731,7 +4745,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
         <v>266</v>
       </c>
@@ -4847,7 +4861,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
         <v>275</v>
       </c>
@@ -4863,7 +4877,7 @@
         <v>78</v>
       </c>
       <c r="G28" t="s" s="2">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="H28" t="s" s="2">
         <v>77</v>
@@ -4958,15 +4972,15 @@
         <v>77</v>
       </c>
       <c r="AN28" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" hidden="true">
+      <c r="A29" t="s" s="2">
         <v>282</v>
       </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s" s="2">
-        <v>283</v>
-      </c>
       <c r="B29" t="s" s="2">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
@@ -4989,13 +5003,13 @@
         <v>87</v>
       </c>
       <c r="K29" t="s" s="2">
+        <v>283</v>
+      </c>
+      <c r="L29" t="s" s="2">
         <v>284</v>
       </c>
-      <c r="L29" t="s" s="2">
+      <c r="M29" t="s" s="2">
         <v>285</v>
-      </c>
-      <c r="M29" t="s" s="2">
-        <v>286</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
@@ -5046,7 +5060,7 @@
         <v>77</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>78</v>
@@ -5061,24 +5075,24 @@
         <v>98</v>
       </c>
       <c r="AK29" t="s" s="2">
+        <v>286</v>
+      </c>
+      <c r="AL29" t="s" s="2">
         <v>287</v>
       </c>
-      <c r="AL29" t="s" s="2">
+      <c r="AM29" t="s" s="2">
         <v>288</v>
       </c>
-      <c r="AM29" t="s" s="2">
+      <c r="AN29" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" hidden="true">
+      <c r="A30" t="s" s="2">
         <v>289</v>
       </c>
-      <c r="AN29" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s" s="2">
-        <v>290</v>
-      </c>
       <c r="B30" t="s" s="2">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -5101,16 +5115,16 @@
         <v>77</v>
       </c>
       <c r="K30" t="s" s="2">
+        <v>290</v>
+      </c>
+      <c r="L30" t="s" s="2">
         <v>291</v>
       </c>
-      <c r="L30" t="s" s="2">
+      <c r="M30" t="s" s="2">
         <v>292</v>
       </c>
-      <c r="M30" t="s" s="2">
+      <c r="N30" t="s" s="2">
         <v>293</v>
-      </c>
-      <c r="N30" t="s" s="2">
-        <v>294</v>
       </c>
       <c r="O30" s="2"/>
       <c r="P30" t="s" s="2">
@@ -5160,7 +5174,7 @@
         <v>77</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>78</v>
@@ -5175,24 +5189,24 @@
         <v>98</v>
       </c>
       <c r="AK30" t="s" s="2">
+        <v>294</v>
+      </c>
+      <c r="AL30" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AM30" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN30" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" hidden="true">
+      <c r="A31" t="s" s="2">
         <v>295</v>
       </c>
-      <c r="AL30" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM30" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN30" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="s" s="2">
-        <v>296</v>
-      </c>
       <c r="B31" t="s" s="2">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -5215,16 +5229,16 @@
         <v>77</v>
       </c>
       <c r="K31" t="s" s="2">
+        <v>296</v>
+      </c>
+      <c r="L31" t="s" s="2">
         <v>297</v>
       </c>
-      <c r="L31" t="s" s="2">
+      <c r="M31" t="s" s="2">
         <v>298</v>
       </c>
-      <c r="M31" t="s" s="2">
+      <c r="N31" t="s" s="2">
         <v>299</v>
-      </c>
-      <c r="N31" t="s" s="2">
-        <v>300</v>
       </c>
       <c r="O31" s="2"/>
       <c r="P31" t="s" s="2">
@@ -5274,7 +5288,7 @@
         <v>77</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>78</v>
@@ -5289,24 +5303,24 @@
         <v>98</v>
       </c>
       <c r="AK31" t="s" s="2">
+        <v>300</v>
+      </c>
+      <c r="AL31" t="s" s="2">
         <v>301</v>
       </c>
-      <c r="AL31" t="s" s="2">
+      <c r="AM31" t="s" s="2">
         <v>302</v>
       </c>
-      <c r="AM31" t="s" s="2">
+      <c r="AN31" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" hidden="true">
+      <c r="A32" t="s" s="2">
         <v>303</v>
       </c>
-      <c r="AN31" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s" s="2">
-        <v>304</v>
-      </c>
       <c r="B32" t="s" s="2">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -5320,7 +5334,7 @@
         <v>86</v>
       </c>
       <c r="H32" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="I32" t="s" s="2">
         <v>77</v>
@@ -5329,13 +5343,13 @@
         <v>77</v>
       </c>
       <c r="K32" t="s" s="2">
+        <v>304</v>
+      </c>
+      <c r="L32" t="s" s="2">
         <v>305</v>
       </c>
-      <c r="L32" t="s" s="2">
+      <c r="M32" t="s" s="2">
         <v>306</v>
-      </c>
-      <c r="M32" t="s" s="2">
-        <v>307</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
@@ -5386,7 +5400,7 @@
         <v>77</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>78</v>
@@ -5401,24 +5415,24 @@
         <v>98</v>
       </c>
       <c r="AK32" t="s" s="2">
+        <v>307</v>
+      </c>
+      <c r="AL32" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AM32" t="s" s="2">
         <v>308</v>
       </c>
-      <c r="AL32" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM32" t="s" s="2">
+      <c r="AN32" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" hidden="true">
+      <c r="A33" t="s" s="2">
         <v>309</v>
       </c>
-      <c r="AN32" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s" s="2">
-        <v>310</v>
-      </c>
       <c r="B33" t="s" s="2">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -5525,12 +5539,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -5639,16 +5653,16 @@
         <v>77</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" t="s" s="2">
@@ -5670,10 +5684,10 @@
         <v>132</v>
       </c>
       <c r="L35" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="M35" t="s" s="2">
         <v>314</v>
-      </c>
-      <c r="M35" t="s" s="2">
-        <v>315</v>
       </c>
       <c r="N35" t="s" s="2">
         <v>135</v>
@@ -5728,7 +5742,7 @@
         <v>77</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>78</v>
@@ -5755,12 +5769,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -5783,13 +5797,13 @@
         <v>87</v>
       </c>
       <c r="K36" t="s" s="2">
+        <v>317</v>
+      </c>
+      <c r="L36" t="s" s="2">
         <v>318</v>
       </c>
-      <c r="L36" t="s" s="2">
+      <c r="M36" t="s" s="2">
         <v>319</v>
-      </c>
-      <c r="M36" t="s" s="2">
-        <v>320</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
@@ -5840,7 +5854,7 @@
         <v>77</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>78</v>
@@ -5855,24 +5869,24 @@
         <v>98</v>
       </c>
       <c r="AK36" t="s" s="2">
+        <v>320</v>
+      </c>
+      <c r="AL36" t="s" s="2">
         <v>321</v>
       </c>
-      <c r="AL36" t="s" s="2">
+      <c r="AM36" t="s" s="2">
         <v>322</v>
       </c>
-      <c r="AM36" t="s" s="2">
+      <c r="AN36" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" hidden="true">
+      <c r="A37" t="s" s="2">
         <v>323</v>
       </c>
-      <c r="AN36" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="s" s="2">
-        <v>324</v>
-      </c>
       <c r="B37" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -5895,13 +5909,13 @@
         <v>87</v>
       </c>
       <c r="K37" t="s" s="2">
+        <v>324</v>
+      </c>
+      <c r="L37" t="s" s="2">
         <v>325</v>
       </c>
-      <c r="L37" t="s" s="2">
+      <c r="M37" t="s" s="2">
         <v>326</v>
-      </c>
-      <c r="M37" t="s" s="2">
-        <v>327</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
@@ -5940,7 +5954,7 @@
         <v>77</v>
       </c>
       <c r="AB37" t="s" s="2">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AC37" s="2"/>
       <c r="AD37" t="s" s="2">
@@ -5950,7 +5964,7 @@
         <v>148</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>78</v>
@@ -5965,27 +5979,27 @@
         <v>98</v>
       </c>
       <c r="AK37" t="s" s="2">
+        <v>328</v>
+      </c>
+      <c r="AL37" t="s" s="2">
         <v>329</v>
       </c>
-      <c r="AL37" t="s" s="2">
+      <c r="AM37" t="s" s="2">
         <v>330</v>
       </c>
-      <c r="AM37" t="s" s="2">
+      <c r="AN37" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" hidden="true">
+      <c r="A38" t="s" s="2">
         <v>331</v>
       </c>
-      <c r="AN37" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="s" s="2">
+      <c r="B38" t="s" s="2">
+        <v>323</v>
+      </c>
+      <c r="C38" t="s" s="2">
         <v>332</v>
-      </c>
-      <c r="B38" t="s" s="2">
-        <v>324</v>
-      </c>
-      <c r="C38" t="s" s="2">
-        <v>333</v>
       </c>
       <c r="D38" t="s" s="2">
         <v>77</v>
@@ -5998,7 +6012,7 @@
         <v>86</v>
       </c>
       <c r="H38" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="I38" t="s" s="2">
         <v>77</v>
@@ -6007,13 +6021,13 @@
         <v>87</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L38" t="s" s="2">
+        <v>325</v>
+      </c>
+      <c r="M38" t="s" s="2">
         <v>326</v>
-      </c>
-      <c r="M38" t="s" s="2">
-        <v>327</v>
       </c>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
@@ -6064,7 +6078,7 @@
         <v>77</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>78</v>
@@ -6079,24 +6093,24 @@
         <v>98</v>
       </c>
       <c r="AK38" t="s" s="2">
+        <v>328</v>
+      </c>
+      <c r="AL38" t="s" s="2">
         <v>329</v>
       </c>
-      <c r="AL38" t="s" s="2">
+      <c r="AM38" t="s" s="2">
         <v>330</v>
       </c>
-      <c r="AM38" t="s" s="2">
-        <v>331</v>
-      </c>
       <c r="AN38" t="s" s="2">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="39" hidden="true">
+      <c r="A39" t="s" s="2">
         <v>334</v>
       </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="s" s="2">
-        <v>335</v>
-      </c>
       <c r="B39" t="s" s="2">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
@@ -6119,13 +6133,13 @@
         <v>87</v>
       </c>
       <c r="K39" t="s" s="2">
+        <v>335</v>
+      </c>
+      <c r="L39" t="s" s="2">
         <v>336</v>
       </c>
-      <c r="L39" t="s" s="2">
+      <c r="M39" t="s" s="2">
         <v>337</v>
-      </c>
-      <c r="M39" t="s" s="2">
-        <v>338</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
@@ -6176,7 +6190,7 @@
         <v>77</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>78</v>
@@ -6194,7 +6208,7 @@
         <v>77</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="AM39" t="s" s="2">
         <v>77</v>
@@ -6203,12 +6217,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -6231,13 +6245,13 @@
         <v>77</v>
       </c>
       <c r="K40" t="s" s="2">
+        <v>339</v>
+      </c>
+      <c r="L40" t="s" s="2">
         <v>340</v>
       </c>
-      <c r="L40" t="s" s="2">
+      <c r="M40" t="s" s="2">
         <v>341</v>
-      </c>
-      <c r="M40" t="s" s="2">
-        <v>342</v>
       </c>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
@@ -6288,7 +6302,7 @@
         <v>77</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>78</v>
@@ -6303,24 +6317,24 @@
         <v>98</v>
       </c>
       <c r="AK40" t="s" s="2">
+        <v>342</v>
+      </c>
+      <c r="AL40" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AM40" t="s" s="2">
         <v>343</v>
       </c>
-      <c r="AL40" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM40" t="s" s="2">
+      <c r="AN40" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" hidden="true">
+      <c r="A41" t="s" s="2">
         <v>344</v>
       </c>
-      <c r="AN40" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="s" s="2">
-        <v>345</v>
-      </c>
       <c r="B41" t="s" s="2">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -6346,10 +6360,10 @@
         <v>182</v>
       </c>
       <c r="L41" t="s" s="2">
+        <v>345</v>
+      </c>
+      <c r="M41" t="s" s="2">
         <v>346</v>
-      </c>
-      <c r="M41" t="s" s="2">
-        <v>347</v>
       </c>
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
@@ -6379,11 +6393,11 @@
         <v>249</v>
       </c>
       <c r="Y41" t="s" s="2">
+        <v>347</v>
+      </c>
+      <c r="Z41" t="s" s="2">
         <v>348</v>
       </c>
-      <c r="Z41" t="s" s="2">
-        <v>349</v>
-      </c>
       <c r="AA41" t="s" s="2">
         <v>77</v>
       </c>
@@ -6400,7 +6414,7 @@
         <v>77</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>78</v>
@@ -6415,24 +6429,24 @@
         <v>98</v>
       </c>
       <c r="AK41" t="s" s="2">
+        <v>349</v>
+      </c>
+      <c r="AL41" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AM41" t="s" s="2">
         <v>350</v>
       </c>
-      <c r="AL41" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM41" t="s" s="2">
+      <c r="AN41" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="42" hidden="true">
+      <c r="A42" t="s" s="2">
         <v>351</v>
       </c>
-      <c r="AN41" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="s" s="2">
-        <v>352</v>
-      </c>
       <c r="B42" t="s" s="2">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -6458,13 +6472,13 @@
         <v>182</v>
       </c>
       <c r="L42" t="s" s="2">
+        <v>352</v>
+      </c>
+      <c r="M42" t="s" s="2">
         <v>353</v>
       </c>
-      <c r="M42" t="s" s="2">
+      <c r="N42" t="s" s="2">
         <v>354</v>
-      </c>
-      <c r="N42" t="s" s="2">
-        <v>355</v>
       </c>
       <c r="O42" s="2"/>
       <c r="P42" t="s" s="2">
@@ -6493,11 +6507,11 @@
         <v>249</v>
       </c>
       <c r="Y42" t="s" s="2">
+        <v>355</v>
+      </c>
+      <c r="Z42" t="s" s="2">
         <v>356</v>
       </c>
-      <c r="Z42" t="s" s="2">
-        <v>357</v>
-      </c>
       <c r="AA42" t="s" s="2">
         <v>77</v>
       </c>
@@ -6514,7 +6528,7 @@
         <v>77</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>78</v>
@@ -6529,24 +6543,24 @@
         <v>98</v>
       </c>
       <c r="AK42" t="s" s="2">
+        <v>357</v>
+      </c>
+      <c r="AL42" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AM42" t="s" s="2">
         <v>358</v>
       </c>
-      <c r="AL42" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM42" t="s" s="2">
+      <c r="AN42" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" hidden="true">
+      <c r="A43" t="s" s="2">
         <v>359</v>
       </c>
-      <c r="AN42" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="s" s="2">
-        <v>360</v>
-      </c>
       <c r="B43" t="s" s="2">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -6569,19 +6583,19 @@
         <v>87</v>
       </c>
       <c r="K43" t="s" s="2">
+        <v>360</v>
+      </c>
+      <c r="L43" t="s" s="2">
         <v>361</v>
       </c>
-      <c r="L43" t="s" s="2">
+      <c r="M43" t="s" s="2">
         <v>362</v>
       </c>
-      <c r="M43" t="s" s="2">
+      <c r="N43" t="s" s="2">
         <v>363</v>
       </c>
-      <c r="N43" t="s" s="2">
+      <c r="O43" t="s" s="2">
         <v>364</v>
-      </c>
-      <c r="O43" t="s" s="2">
-        <v>365</v>
       </c>
       <c r="P43" t="s" s="2">
         <v>77</v>
@@ -6609,11 +6623,11 @@
         <v>187</v>
       </c>
       <c r="Y43" t="s" s="2">
+        <v>365</v>
+      </c>
+      <c r="Z43" t="s" s="2">
         <v>366</v>
       </c>
-      <c r="Z43" t="s" s="2">
-        <v>367</v>
-      </c>
       <c r="AA43" t="s" s="2">
         <v>77</v>
       </c>
@@ -6630,7 +6644,7 @@
         <v>77</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>78</v>
@@ -6651,18 +6665,18 @@
         <v>77</v>
       </c>
       <c r="AM43" t="s" s="2">
+        <v>367</v>
+      </c>
+      <c r="AN43" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="44" hidden="true">
+      <c r="A44" t="s" s="2">
         <v>368</v>
       </c>
-      <c r="AN43" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="s" s="2">
-        <v>369</v>
-      </c>
       <c r="B44" t="s" s="2">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -6685,13 +6699,13 @@
         <v>77</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="L44" t="s" s="2">
+        <v>369</v>
+      </c>
+      <c r="M44" t="s" s="2">
         <v>370</v>
-      </c>
-      <c r="M44" t="s" s="2">
-        <v>371</v>
       </c>
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
@@ -6742,7 +6756,7 @@
         <v>77</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>78</v>
@@ -6757,24 +6771,24 @@
         <v>98</v>
       </c>
       <c r="AK44" t="s" s="2">
+        <v>371</v>
+      </c>
+      <c r="AL44" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AM44" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN44" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="45" hidden="true">
+      <c r="A45" t="s" s="2">
         <v>372</v>
       </c>
-      <c r="AL44" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM44" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN44" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="s" s="2">
-        <v>373</v>
-      </c>
       <c r="B45" t="s" s="2">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -6881,12 +6895,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
@@ -6995,16 +7009,16 @@
         <v>77</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" t="s" s="2">
@@ -7026,10 +7040,10 @@
         <v>132</v>
       </c>
       <c r="L47" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="M47" t="s" s="2">
         <v>314</v>
-      </c>
-      <c r="M47" t="s" s="2">
-        <v>315</v>
       </c>
       <c r="N47" t="s" s="2">
         <v>135</v>
@@ -7084,7 +7098,7 @@
         <v>77</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>78</v>
@@ -7111,12 +7125,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -7142,10 +7156,10 @@
         <v>157</v>
       </c>
       <c r="L48" t="s" s="2">
+        <v>376</v>
+      </c>
+      <c r="M48" t="s" s="2">
         <v>377</v>
-      </c>
-      <c r="M48" t="s" s="2">
-        <v>378</v>
       </c>
       <c r="N48" s="2"/>
       <c r="O48" s="2"/>
@@ -7196,7 +7210,7 @@
         <v>77</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>78</v>
@@ -7211,24 +7225,24 @@
         <v>98</v>
       </c>
       <c r="AK48" t="s" s="2">
+        <v>378</v>
+      </c>
+      <c r="AL48" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AM48" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN48" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="49" hidden="true">
+      <c r="A49" t="s" s="2">
         <v>379</v>
       </c>
-      <c r="AL48" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM48" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN48" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="s" s="2">
-        <v>380</v>
-      </c>
       <c r="B49" t="s" s="2">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
@@ -7254,10 +7268,10 @@
         <v>182</v>
       </c>
       <c r="L49" t="s" s="2">
+        <v>380</v>
+      </c>
+      <c r="M49" t="s" s="2">
         <v>381</v>
-      </c>
-      <c r="M49" t="s" s="2">
-        <v>382</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" s="2"/>
@@ -7287,11 +7301,11 @@
         <v>249</v>
       </c>
       <c r="Y49" t="s" s="2">
+        <v>382</v>
+      </c>
+      <c r="Z49" t="s" s="2">
         <v>383</v>
       </c>
-      <c r="Z49" t="s" s="2">
-        <v>384</v>
-      </c>
       <c r="AA49" t="s" s="2">
         <v>77</v>
       </c>
@@ -7308,7 +7322,7 @@
         <v>77</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>78</v>
@@ -7335,12 +7349,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
@@ -7363,13 +7377,13 @@
         <v>77</v>
       </c>
       <c r="K50" t="s" s="2">
+        <v>385</v>
+      </c>
+      <c r="L50" t="s" s="2">
         <v>386</v>
       </c>
-      <c r="L50" t="s" s="2">
+      <c r="M50" t="s" s="2">
         <v>387</v>
-      </c>
-      <c r="M50" t="s" s="2">
-        <v>388</v>
       </c>
       <c r="N50" s="2"/>
       <c r="O50" s="2"/>
@@ -7420,7 +7434,7 @@
         <v>77</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>78</v>
@@ -7435,24 +7449,24 @@
         <v>98</v>
       </c>
       <c r="AK50" t="s" s="2">
+        <v>388</v>
+      </c>
+      <c r="AL50" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AM50" t="s" s="2">
         <v>389</v>
       </c>
-      <c r="AL50" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM50" t="s" s="2">
+      <c r="AN50" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="51" hidden="true">
+      <c r="A51" t="s" s="2">
         <v>390</v>
       </c>
-      <c r="AN50" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="s" s="2">
-        <v>391</v>
-      </c>
       <c r="B51" t="s" s="2">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
@@ -7475,13 +7489,13 @@
         <v>77</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="L51" t="s" s="2">
+        <v>391</v>
+      </c>
+      <c r="M51" t="s" s="2">
         <v>392</v>
-      </c>
-      <c r="M51" t="s" s="2">
-        <v>393</v>
       </c>
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
@@ -7532,7 +7546,7 @@
         <v>77</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>78</v>
@@ -7547,7 +7561,7 @@
         <v>98</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="AL51" t="s" s="2">
         <v>77</v>
@@ -7559,12 +7573,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
@@ -7587,13 +7601,13 @@
         <v>77</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="L52" t="s" s="2">
+        <v>394</v>
+      </c>
+      <c r="M52" t="s" s="2">
         <v>395</v>
-      </c>
-      <c r="M52" t="s" s="2">
-        <v>396</v>
       </c>
       <c r="N52" s="2"/>
       <c r="O52" s="2"/>
@@ -7644,7 +7658,7 @@
         <v>77</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>78</v>
@@ -7659,24 +7673,24 @@
         <v>98</v>
       </c>
       <c r="AK52" t="s" s="2">
+        <v>396</v>
+      </c>
+      <c r="AL52" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AM52" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN52" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="53" hidden="true">
+      <c r="A53" t="s" s="2">
         <v>397</v>
       </c>
-      <c r="AL52" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM52" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN52" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="s" s="2">
-        <v>398</v>
-      </c>
       <c r="B53" t="s" s="2">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
@@ -7783,12 +7797,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" t="s" s="2">
@@ -7897,16 +7911,16 @@
         <v>77</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" t="s" s="2">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" t="s" s="2">
@@ -7928,10 +7942,10 @@
         <v>132</v>
       </c>
       <c r="L55" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="M55" t="s" s="2">
         <v>314</v>
-      </c>
-      <c r="M55" t="s" s="2">
-        <v>315</v>
       </c>
       <c r="N55" t="s" s="2">
         <v>135</v>
@@ -7986,7 +8000,7 @@
         <v>77</v>
       </c>
       <c r="AF55" t="s" s="2">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AG55" t="s" s="2">
         <v>78</v>
@@ -8013,12 +8027,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" t="s" s="2">
@@ -8044,10 +8058,10 @@
         <v>144</v>
       </c>
       <c r="L56" t="s" s="2">
+        <v>401</v>
+      </c>
+      <c r="M56" t="s" s="2">
         <v>402</v>
-      </c>
-      <c r="M56" t="s" s="2">
-        <v>403</v>
       </c>
       <c r="N56" s="2"/>
       <c r="O56" s="2"/>
@@ -8098,7 +8112,7 @@
         <v>77</v>
       </c>
       <c r="AF56" t="s" s="2">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="AG56" t="s" s="2">
         <v>78</v>
@@ -8119,18 +8133,18 @@
         <v>77</v>
       </c>
       <c r="AM56" t="s" s="2">
+        <v>403</v>
+      </c>
+      <c r="AN56" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="57" hidden="true">
+      <c r="A57" t="s" s="2">
         <v>404</v>
       </c>
-      <c r="AN56" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="s" s="2">
-        <v>405</v>
-      </c>
       <c r="B57" t="s" s="2">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" t="s" s="2">
@@ -8156,10 +8170,10 @@
         <v>157</v>
       </c>
       <c r="L57" t="s" s="2">
+        <v>405</v>
+      </c>
+      <c r="M57" t="s" s="2">
         <v>406</v>
-      </c>
-      <c r="M57" t="s" s="2">
-        <v>407</v>
       </c>
       <c r="N57" s="2"/>
       <c r="O57" s="2"/>
@@ -8210,7 +8224,7 @@
         <v>77</v>
       </c>
       <c r="AF57" t="s" s="2">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="AG57" t="s" s="2">
         <v>78</v>
@@ -8225,24 +8239,24 @@
         <v>98</v>
       </c>
       <c r="AK57" t="s" s="2">
+        <v>407</v>
+      </c>
+      <c r="AL57" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AM57" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN57" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="58" hidden="true">
+      <c r="A58" t="s" s="2">
         <v>408</v>
       </c>
-      <c r="AL57" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM57" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN57" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="s" s="2">
-        <v>409</v>
-      </c>
       <c r="B58" t="s" s="2">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" t="s" s="2">
@@ -8268,10 +8282,10 @@
         <v>182</v>
       </c>
       <c r="L58" t="s" s="2">
+        <v>409</v>
+      </c>
+      <c r="M58" t="s" s="2">
         <v>410</v>
-      </c>
-      <c r="M58" t="s" s="2">
-        <v>411</v>
       </c>
       <c r="N58" s="2"/>
       <c r="O58" s="2"/>
@@ -8301,11 +8315,11 @@
         <v>249</v>
       </c>
       <c r="Y58" t="s" s="2">
+        <v>411</v>
+      </c>
+      <c r="Z58" t="s" s="2">
         <v>412</v>
       </c>
-      <c r="Z58" t="s" s="2">
-        <v>413</v>
-      </c>
       <c r="AA58" t="s" s="2">
         <v>77</v>
       </c>
@@ -8322,7 +8336,7 @@
         <v>77</v>
       </c>
       <c r="AF58" t="s" s="2">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="AG58" t="s" s="2">
         <v>78</v>
@@ -8343,18 +8357,18 @@
         <v>77</v>
       </c>
       <c r="AM58" t="s" s="2">
+        <v>413</v>
+      </c>
+      <c r="AN58" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="59" hidden="true">
+      <c r="A59" t="s" s="2">
         <v>414</v>
       </c>
-      <c r="AN58" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="s" s="2">
-        <v>415</v>
-      </c>
       <c r="B59" t="s" s="2">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s" s="2">
@@ -8377,13 +8391,13 @@
         <v>77</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="L59" t="s" s="2">
+        <v>415</v>
+      </c>
+      <c r="M59" t="s" s="2">
         <v>416</v>
-      </c>
-      <c r="M59" t="s" s="2">
-        <v>417</v>
       </c>
       <c r="N59" s="2"/>
       <c r="O59" s="2"/>
@@ -8434,7 +8448,7 @@
         <v>77</v>
       </c>
       <c r="AF59" t="s" s="2">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="AG59" t="s" s="2">
         <v>78</v>
@@ -8449,24 +8463,24 @@
         <v>98</v>
       </c>
       <c r="AK59" t="s" s="2">
+        <v>417</v>
+      </c>
+      <c r="AL59" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AM59" t="s" s="2">
         <v>418</v>
       </c>
-      <c r="AL59" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM59" t="s" s="2">
+      <c r="AN59" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="60" hidden="true">
+      <c r="A60" t="s" s="2">
         <v>419</v>
       </c>
-      <c r="AN59" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="s" s="2">
-        <v>420</v>
-      </c>
       <c r="B60" t="s" s="2">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" t="s" s="2">
@@ -8489,13 +8503,13 @@
         <v>77</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="L60" t="s" s="2">
+        <v>420</v>
+      </c>
+      <c r="M60" t="s" s="2">
         <v>421</v>
-      </c>
-      <c r="M60" t="s" s="2">
-        <v>422</v>
       </c>
       <c r="N60" s="2"/>
       <c r="O60" s="2"/>
@@ -8546,7 +8560,7 @@
         <v>77</v>
       </c>
       <c r="AF60" t="s" s="2">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="AG60" t="s" s="2">
         <v>78</v>
@@ -8561,24 +8575,24 @@
         <v>98</v>
       </c>
       <c r="AK60" t="s" s="2">
+        <v>422</v>
+      </c>
+      <c r="AL60" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AM60" t="s" s="2">
         <v>423</v>
       </c>
-      <c r="AL60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM60" t="s" s="2">
+      <c r="AN60" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="61" hidden="true">
+      <c r="A61" t="s" s="2">
         <v>424</v>
       </c>
-      <c r="AN60" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="s" s="2">
-        <v>425</v>
-      </c>
       <c r="B61" t="s" s="2">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" t="s" s="2">
@@ -8601,13 +8615,13 @@
         <v>77</v>
       </c>
       <c r="K61" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="L61" t="s" s="2">
         <v>426</v>
       </c>
-      <c r="L61" t="s" s="2">
+      <c r="M61" t="s" s="2">
         <v>427</v>
-      </c>
-      <c r="M61" t="s" s="2">
-        <v>428</v>
       </c>
       <c r="N61" s="2"/>
       <c r="O61" s="2"/>
@@ -8637,11 +8651,11 @@
         <v>249</v>
       </c>
       <c r="Y61" t="s" s="2">
+        <v>428</v>
+      </c>
+      <c r="Z61" t="s" s="2">
         <v>429</v>
       </c>
-      <c r="Z61" t="s" s="2">
-        <v>430</v>
-      </c>
       <c r="AA61" t="s" s="2">
         <v>77</v>
       </c>
@@ -8658,7 +8672,7 @@
         <v>77</v>
       </c>
       <c r="AF61" t="s" s="2">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="AG61" t="s" s="2">
         <v>78</v>
@@ -8673,24 +8687,24 @@
         <v>98</v>
       </c>
       <c r="AK61" t="s" s="2">
+        <v>430</v>
+      </c>
+      <c r="AL61" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AM61" t="s" s="2">
         <v>431</v>
       </c>
-      <c r="AL61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM61" t="s" s="2">
+      <c r="AN61" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="62" hidden="true">
+      <c r="A62" t="s" s="2">
         <v>432</v>
       </c>
-      <c r="AN61" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="s" s="2">
-        <v>433</v>
-      </c>
       <c r="B62" t="s" s="2">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" t="s" s="2">
@@ -8716,16 +8730,16 @@
         <v>182</v>
       </c>
       <c r="L62" t="s" s="2">
+        <v>433</v>
+      </c>
+      <c r="M62" t="s" s="2">
         <v>434</v>
       </c>
-      <c r="M62" t="s" s="2">
+      <c r="N62" t="s" s="2">
         <v>435</v>
       </c>
-      <c r="N62" t="s" s="2">
+      <c r="O62" t="s" s="2">
         <v>436</v>
-      </c>
-      <c r="O62" t="s" s="2">
-        <v>437</v>
       </c>
       <c r="P62" t="s" s="2">
         <v>77</v>
@@ -8753,11 +8767,11 @@
         <v>187</v>
       </c>
       <c r="Y62" t="s" s="2">
+        <v>437</v>
+      </c>
+      <c r="Z62" t="s" s="2">
         <v>438</v>
       </c>
-      <c r="Z62" t="s" s="2">
-        <v>439</v>
-      </c>
       <c r="AA62" t="s" s="2">
         <v>77</v>
       </c>
@@ -8774,7 +8788,7 @@
         <v>77</v>
       </c>
       <c r="AF62" t="s" s="2">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="AG62" t="s" s="2">
         <v>78</v>
@@ -8795,18 +8809,18 @@
         <v>77</v>
       </c>
       <c r="AM62" t="s" s="2">
+        <v>439</v>
+      </c>
+      <c r="AN62" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="63" hidden="true">
+      <c r="A63" t="s" s="2">
         <v>440</v>
       </c>
-      <c r="AN62" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="s" s="2">
-        <v>441</v>
-      </c>
       <c r="B63" t="s" s="2">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" t="s" s="2">
@@ -8829,13 +8843,13 @@
         <v>77</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="L63" t="s" s="2">
         <v>50</v>
       </c>
       <c r="M63" t="s" s="2">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="N63" s="2"/>
       <c r="O63" s="2"/>
@@ -8886,7 +8900,7 @@
         <v>77</v>
       </c>
       <c r="AF63" t="s" s="2">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="AG63" t="s" s="2">
         <v>78</v>
@@ -8901,19 +8915,37 @@
         <v>98</v>
       </c>
       <c r="AK63" t="s" s="2">
+        <v>443</v>
+      </c>
+      <c r="AL63" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AM63" t="s" s="2">
         <v>444</v>
-      </c>
-      <c r="AL63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM63" t="s" s="2">
-        <v>445</v>
       </c>
       <c r="AN63" t="s" s="2">
         <v>77</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AN63">
+    <filterColumn colId="6">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+    <filterColumn colId="26">
+      <filters blank="true"/>
+    </filterColumn>
+  </autoFilter>
+  <conditionalFormatting sqref="A2:AI62">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$G2&lt;&gt;"Y"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$Q2&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add example of CBC report
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-VA.MHV.PHR.LabSpecimen.xlsx
+++ b/docs/StructureDefinition-VA.MHV.PHR.LabSpecimen.xlsx
@@ -10,13 +10,13 @@
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AN$63</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AN$59</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2290" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2145" uniqueCount="426">
   <si>
     <t>Property</t>
   </si>
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.7-beta</t>
+    <t>0.1.8-beta</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-04-11T08:45:33-05:00</t>
+    <t>2023-04-12T10:49:54-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -817,65 +817,7 @@
     <t>SPM-4 and possibly SPM-5</t>
   </si>
   <si>
-    <t>Specimen.type.id</t>
-  </si>
-  <si>
-    <t>Specimen.type.extension</t>
-  </si>
-  <si>
-    <t>Specimen.type.coding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coding
-</t>
-  </si>
-  <si>
-    <t>Code defined by a terminology system</t>
-  </si>
-  <si>
-    <t>A reference to a code defined by a terminology system.</t>
-  </si>
-  <si>
-    <t>Codes may be defined very casually in enumerations, or code lists, up to very formal definitions such as SNOMED CT - see the HL7 v3 Core Principles for more information.  Ordering of codings is undefined and SHALL NOT be used to infer meaning. Generally, at most only one of the coding values will be labeled as UserSelected = true.</t>
-  </si>
-  <si>
-    <t>Allows for alternative encodings within a code system, and translations to other code systems.</t>
-  </si>
-  <si>
-    <t>CodeableConcept.coding</t>
-  </si>
-  <si>
-    <t>union(., ./translation)</t>
-  </si>
-  <si>
-    <t>C*E.1-8, C*E.10-22</t>
-  </si>
-  <si>
-    <t>Specimen.type.text</t>
-  </si>
-  <si>
-    <t>Plain text representation of the concept</t>
-  </si>
-  <si>
-    <t>A human language representation of the concept as seen/selected/uttered by the user who entered the data and/or which represents the intended meaning of the user.</t>
-  </si>
-  <si>
-    <t>Very often the text is the same as a displayName of one of the codings.</t>
-  </si>
-  <si>
-    <t>The codes from the terminologies do not always capture the correct meaning with all the nuances of the human using them, or sometimes there is no appropriate code at all. In these cases, the text is used to capture the full meaning of the source.</t>
-  </si>
-  <si>
-    <t>CodeableConcept.text</t>
-  </si>
-  <si>
-    <t>./originalText[mediaType/code="text/plain"]/data</t>
-  </si>
-  <si>
-    <t>C*E.9. But note many systems use C*E.2 for this</t>
-  </si>
-  <si>
-    <t>LabSpecimenTO.name</t>
+    <t>text = LabSpecimenTO.name</t>
   </si>
   <si>
     <t>Specimen.subject</t>
@@ -1729,7 +1671,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AN63"/>
+  <dimension ref="A1:AN59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -4400,15 +4342,15 @@
         <v>254</v>
       </c>
       <c r="AN23" t="s" s="2">
-        <v>77</v>
+        <v>255</v>
       </c>
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
@@ -4419,7 +4361,7 @@
         <v>78</v>
       </c>
       <c r="G24" t="s" s="2">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="H24" t="s" s="2">
         <v>77</v>
@@ -4428,19 +4370,21 @@
         <v>77</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>157</v>
+        <v>257</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>158</v>
+        <v>258</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>159</v>
+        <v>259</v>
       </c>
       <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
+      <c r="O24" t="s" s="2">
+        <v>260</v>
+      </c>
       <c r="P24" t="s" s="2">
         <v>77</v>
       </c>
@@ -4488,7 +4432,7 @@
         <v>77</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>160</v>
+        <v>256</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>78</v>
@@ -4500,13 +4444,13 @@
         <v>77</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>161</v>
+        <v>261</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>77</v>
+        <v>262</v>
       </c>
       <c r="AM24" t="s" s="2">
         <v>77</v>
@@ -4517,21 +4461,21 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
-        <v>131</v>
+        <v>77</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G25" t="s" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H25" t="s" s="2">
         <v>77</v>
@@ -4540,20 +4484,18 @@
         <v>77</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>132</v>
+        <v>264</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>133</v>
+        <v>265</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>164</v>
-      </c>
-      <c r="N25" t="s" s="2">
-        <v>135</v>
-      </c>
+        <v>266</v>
+      </c>
+      <c r="N25" s="2"/>
       <c r="O25" s="2"/>
       <c r="P25" t="s" s="2">
         <v>77</v>
@@ -4590,40 +4532,40 @@
         <v>77</v>
       </c>
       <c r="AB25" t="s" s="2">
-        <v>165</v>
+        <v>77</v>
       </c>
       <c r="AC25" t="s" s="2">
-        <v>166</v>
+        <v>77</v>
       </c>
       <c r="AD25" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>148</v>
+        <v>77</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>167</v>
+        <v>263</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH25" t="s" s="2">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="AI25" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>137</v>
+        <v>98</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>161</v>
+        <v>267</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>77</v>
+        <v>268</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>77</v>
+        <v>269</v>
       </c>
       <c r="AN25" t="s" s="2">
         <v>77</v>
@@ -4631,10 +4573,10 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>257</v>
+        <v>270</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>257</v>
+        <v>270</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
@@ -4645,7 +4587,7 @@
         <v>78</v>
       </c>
       <c r="G26" t="s" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H26" t="s" s="2">
         <v>77</v>
@@ -4654,23 +4596,21 @@
         <v>77</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>258</v>
+        <v>271</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>259</v>
+        <v>272</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>260</v>
+        <v>273</v>
       </c>
       <c r="N26" t="s" s="2">
-        <v>261</v>
-      </c>
-      <c r="O26" t="s" s="2">
-        <v>262</v>
-      </c>
+        <v>274</v>
+      </c>
+      <c r="O26" s="2"/>
       <c r="P26" t="s" s="2">
         <v>77</v>
       </c>
@@ -4718,7 +4658,7 @@
         <v>77</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>78</v>
@@ -4733,13 +4673,13 @@
         <v>98</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>264</v>
+        <v>275</v>
       </c>
       <c r="AL26" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>265</v>
+        <v>77</v>
       </c>
       <c r="AN26" t="s" s="2">
         <v>77</v>
@@ -4747,10 +4687,10 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>266</v>
+        <v>276</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>266</v>
+        <v>276</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
@@ -4761,7 +4701,7 @@
         <v>78</v>
       </c>
       <c r="G27" t="s" s="2">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="H27" t="s" s="2">
         <v>77</v>
@@ -4770,23 +4710,21 @@
         <v>77</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>157</v>
+        <v>277</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>267</v>
+        <v>278</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>268</v>
+        <v>279</v>
       </c>
       <c r="N27" t="s" s="2">
-        <v>269</v>
-      </c>
-      <c r="O27" t="s" s="2">
-        <v>270</v>
-      </c>
+        <v>280</v>
+      </c>
+      <c r="O27" s="2"/>
       <c r="P27" t="s" s="2">
         <v>77</v>
       </c>
@@ -4834,13 +4772,13 @@
         <v>77</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH27" t="s" s="2">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AI27" t="s" s="2">
         <v>77</v>
@@ -4849,24 +4787,24 @@
         <v>98</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>272</v>
+        <v>281</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>77</v>
+        <v>282</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>273</v>
+        <v>283</v>
       </c>
       <c r="AN27" t="s" s="2">
-        <v>274</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
@@ -4877,30 +4815,28 @@
         <v>78</v>
       </c>
       <c r="G28" t="s" s="2">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="H28" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="I28" t="s" s="2">
         <v>77</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>277</v>
+        <v>286</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>278</v>
+        <v>287</v>
       </c>
       <c r="N28" s="2"/>
-      <c r="O28" t="s" s="2">
-        <v>279</v>
-      </c>
+      <c r="O28" s="2"/>
       <c r="P28" t="s" s="2">
         <v>77</v>
       </c>
@@ -4948,7 +4884,7 @@
         <v>77</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>78</v>
@@ -4963,13 +4899,13 @@
         <v>98</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>281</v>
+        <v>77</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>77</v>
+        <v>289</v>
       </c>
       <c r="AN28" t="s" s="2">
         <v>77</v>
@@ -4977,10 +4913,10 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
@@ -4991,7 +4927,7 @@
         <v>78</v>
       </c>
       <c r="G29" t="s" s="2">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="H29" t="s" s="2">
         <v>77</v>
@@ -5000,16 +4936,16 @@
         <v>77</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>283</v>
+        <v>157</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>284</v>
+        <v>158</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>285</v>
+        <v>159</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
@@ -5060,7 +4996,7 @@
         <v>77</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>282</v>
+        <v>160</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>78</v>
@@ -5072,16 +5008,16 @@
         <v>77</v>
       </c>
       <c r="AJ29" t="s" s="2">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>286</v>
+        <v>161</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>287</v>
+        <v>77</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>288</v>
+        <v>77</v>
       </c>
       <c r="AN29" t="s" s="2">
         <v>77</v>
@@ -5089,21 +5025,21 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
-        <v>77</v>
+        <v>131</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G30" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H30" t="s" s="2">
         <v>77</v>
@@ -5115,16 +5051,16 @@
         <v>77</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>290</v>
+        <v>132</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>291</v>
+        <v>133</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>292</v>
+        <v>164</v>
       </c>
       <c r="N30" t="s" s="2">
-        <v>293</v>
+        <v>135</v>
       </c>
       <c r="O30" s="2"/>
       <c r="P30" t="s" s="2">
@@ -5174,7 +5110,7 @@
         <v>77</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>289</v>
+        <v>167</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>78</v>
@@ -5186,10 +5122,10 @@
         <v>77</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>98</v>
+        <v>137</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>294</v>
+        <v>161</v>
       </c>
       <c r="AL30" t="s" s="2">
         <v>77</v>
@@ -5203,44 +5139,46 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
-        <v>77</v>
+        <v>293</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G31" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H31" t="s" s="2">
         <v>77</v>
       </c>
       <c r="I31" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>296</v>
+        <v>132</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="N31" t="s" s="2">
-        <v>299</v>
-      </c>
-      <c r="O31" s="2"/>
+        <v>135</v>
+      </c>
+      <c r="O31" t="s" s="2">
+        <v>141</v>
+      </c>
       <c r="P31" t="s" s="2">
         <v>77</v>
       </c>
@@ -5288,7 +5226,7 @@
         <v>77</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>78</v>
@@ -5300,16 +5238,16 @@
         <v>77</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>98</v>
+        <v>137</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>300</v>
+        <v>129</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>301</v>
+        <v>77</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>302</v>
+        <v>77</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>77</v>
@@ -5317,10 +5255,10 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -5331,25 +5269,25 @@
         <v>78</v>
       </c>
       <c r="G32" t="s" s="2">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="H32" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I32" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="J32" t="s" s="2">
         <v>87</v>
       </c>
-      <c r="I32" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="J32" t="s" s="2">
-        <v>77</v>
-      </c>
       <c r="K32" t="s" s="2">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
@@ -5400,7 +5338,7 @@
         <v>77</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>78</v>
@@ -5415,13 +5353,13 @@
         <v>98</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>77</v>
+        <v>302</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>77</v>
@@ -5429,10 +5367,10 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -5452,16 +5390,16 @@
         <v>77</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>157</v>
+        <v>305</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>158</v>
+        <v>306</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>159</v>
+        <v>307</v>
       </c>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
@@ -5500,19 +5438,17 @@
         <v>77</v>
       </c>
       <c r="AB33" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC33" t="s" s="2">
-        <v>77</v>
-      </c>
+        <v>308</v>
+      </c>
+      <c r="AC33" s="2"/>
       <c r="AD33" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>77</v>
+        <v>148</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>160</v>
+        <v>304</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>78</v>
@@ -5524,16 +5460,16 @@
         <v>77</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>161</v>
+        <v>309</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>77</v>
+        <v>310</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>77</v>
+        <v>311</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>77</v>
@@ -5541,43 +5477,43 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>310</v>
-      </c>
-      <c r="C34" s="2"/>
+        <v>304</v>
+      </c>
+      <c r="C34" t="s" s="2">
+        <v>313</v>
+      </c>
       <c r="D34" t="s" s="2">
-        <v>131</v>
+        <v>77</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G34" t="s" s="2">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="H34" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="I34" t="s" s="2">
         <v>77</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>132</v>
+        <v>264</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>133</v>
+        <v>306</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>164</v>
-      </c>
-      <c r="N34" t="s" s="2">
-        <v>135</v>
-      </c>
+        <v>307</v>
+      </c>
+      <c r="N34" s="2"/>
       <c r="O34" s="2"/>
       <c r="P34" t="s" s="2">
         <v>77</v>
@@ -5626,75 +5562,71 @@
         <v>77</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>167</v>
+        <v>304</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH34" t="s" s="2">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="AI34" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>137</v>
+        <v>98</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>161</v>
+        <v>309</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>77</v>
+        <v>310</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>77</v>
+        <v>311</v>
       </c>
       <c r="AN34" t="s" s="2">
-        <v>77</v>
+        <v>314</v>
       </c>
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
-        <v>312</v>
+        <v>77</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G35" t="s" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H35" t="s" s="2">
         <v>77</v>
       </c>
       <c r="I35" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="J35" t="s" s="2">
         <v>87</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>132</v>
+        <v>316</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>314</v>
-      </c>
-      <c r="N35" t="s" s="2">
-        <v>135</v>
-      </c>
-      <c r="O35" t="s" s="2">
-        <v>141</v>
-      </c>
+        <v>318</v>
+      </c>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
       <c r="P35" t="s" s="2">
         <v>77</v>
       </c>
@@ -5748,19 +5680,19 @@
         <v>78</v>
       </c>
       <c r="AH35" t="s" s="2">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="AI35" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>137</v>
+        <v>98</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>129</v>
+        <v>77</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>77</v>
+        <v>310</v>
       </c>
       <c r="AM35" t="s" s="2">
         <v>77</v>
@@ -5771,10 +5703,10 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -5794,16 +5726,16 @@
         <v>77</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
@@ -5854,7 +5786,7 @@
         <v>77</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>78</v>
@@ -5869,13 +5801,13 @@
         <v>98</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>321</v>
+        <v>77</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="AN36" t="s" s="2">
         <v>77</v>
@@ -5883,10 +5815,10 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -5897,7 +5829,7 @@
         <v>78</v>
       </c>
       <c r="G37" t="s" s="2">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="H37" t="s" s="2">
         <v>77</v>
@@ -5906,16 +5838,16 @@
         <v>77</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>324</v>
+        <v>182</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
@@ -5942,29 +5874,31 @@
         <v>77</v>
       </c>
       <c r="X37" t="s" s="2">
-        <v>77</v>
+        <v>249</v>
       </c>
       <c r="Y37" t="s" s="2">
-        <v>77</v>
+        <v>328</v>
       </c>
       <c r="Z37" t="s" s="2">
-        <v>77</v>
+        <v>329</v>
       </c>
       <c r="AA37" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AB37" t="s" s="2">
-        <v>327</v>
-      </c>
-      <c r="AC37" s="2"/>
+        <v>77</v>
+      </c>
+      <c r="AC37" t="s" s="2">
+        <v>77</v>
+      </c>
       <c r="AD37" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>148</v>
+        <v>77</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>78</v>
@@ -5979,13 +5913,13 @@
         <v>98</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>329</v>
+        <v>77</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>77</v>
@@ -5993,14 +5927,12 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>323</v>
-      </c>
-      <c r="C38" t="s" s="2">
         <v>332</v>
       </c>
+      <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
         <v>77</v>
       </c>
@@ -6009,27 +5941,29 @@
         <v>78</v>
       </c>
       <c r="G38" t="s" s="2">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="H38" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="I38" t="s" s="2">
         <v>77</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>283</v>
+        <v>182</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>325</v>
+        <v>333</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>326</v>
-      </c>
-      <c r="N38" s="2"/>
+        <v>334</v>
+      </c>
+      <c r="N38" t="s" s="2">
+        <v>335</v>
+      </c>
       <c r="O38" s="2"/>
       <c r="P38" t="s" s="2">
         <v>77</v>
@@ -6054,13 +5988,13 @@
         <v>77</v>
       </c>
       <c r="X38" t="s" s="2">
-        <v>77</v>
+        <v>249</v>
       </c>
       <c r="Y38" t="s" s="2">
-        <v>77</v>
+        <v>336</v>
       </c>
       <c r="Z38" t="s" s="2">
-        <v>77</v>
+        <v>337</v>
       </c>
       <c r="AA38" t="s" s="2">
         <v>77</v>
@@ -6078,7 +6012,7 @@
         <v>77</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>323</v>
+        <v>332</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>78</v>
@@ -6093,24 +6027,24 @@
         <v>98</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>328</v>
+        <v>338</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>329</v>
+        <v>77</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>330</v>
+        <v>339</v>
       </c>
       <c r="AN38" t="s" s="2">
-        <v>333</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
@@ -6133,16 +6067,20 @@
         <v>87</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>335</v>
+        <v>341</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>336</v>
+        <v>342</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>337</v>
-      </c>
-      <c r="N39" s="2"/>
-      <c r="O39" s="2"/>
+        <v>343</v>
+      </c>
+      <c r="N39" t="s" s="2">
+        <v>344</v>
+      </c>
+      <c r="O39" t="s" s="2">
+        <v>345</v>
+      </c>
       <c r="P39" t="s" s="2">
         <v>77</v>
       </c>
@@ -6166,13 +6104,13 @@
         <v>77</v>
       </c>
       <c r="X39" t="s" s="2">
-        <v>77</v>
+        <v>187</v>
       </c>
       <c r="Y39" t="s" s="2">
-        <v>77</v>
+        <v>346</v>
       </c>
       <c r="Z39" t="s" s="2">
-        <v>77</v>
+        <v>347</v>
       </c>
       <c r="AA39" t="s" s="2">
         <v>77</v>
@@ -6190,7 +6128,7 @@
         <v>77</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>78</v>
@@ -6208,10 +6146,10 @@
         <v>77</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>329</v>
+        <v>77</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>77</v>
+        <v>348</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>77</v>
@@ -6219,10 +6157,10 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>338</v>
+        <v>349</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>338</v>
+        <v>349</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -6245,13 +6183,13 @@
         <v>77</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>339</v>
+        <v>285</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>340</v>
+        <v>350</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>341</v>
+        <v>351</v>
       </c>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
@@ -6302,13 +6240,13 @@
         <v>77</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>338</v>
+        <v>349</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH40" t="s" s="2">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AI40" t="s" s="2">
         <v>77</v>
@@ -6317,13 +6255,13 @@
         <v>98</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="AL40" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>343</v>
+        <v>77</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>77</v>
@@ -6331,10 +6269,10 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>344</v>
+        <v>353</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>344</v>
+        <v>353</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -6345,7 +6283,7 @@
         <v>78</v>
       </c>
       <c r="G41" t="s" s="2">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="H41" t="s" s="2">
         <v>77</v>
@@ -6357,13 +6295,13 @@
         <v>77</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>182</v>
+        <v>157</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>345</v>
+        <v>158</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>346</v>
+        <v>159</v>
       </c>
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
@@ -6390,13 +6328,13 @@
         <v>77</v>
       </c>
       <c r="X41" t="s" s="2">
-        <v>249</v>
+        <v>77</v>
       </c>
       <c r="Y41" t="s" s="2">
-        <v>347</v>
+        <v>77</v>
       </c>
       <c r="Z41" t="s" s="2">
-        <v>348</v>
+        <v>77</v>
       </c>
       <c r="AA41" t="s" s="2">
         <v>77</v>
@@ -6414,7 +6352,7 @@
         <v>77</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>344</v>
+        <v>160</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>78</v>
@@ -6426,16 +6364,16 @@
         <v>77</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>349</v>
+        <v>161</v>
       </c>
       <c r="AL41" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>350</v>
+        <v>77</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>77</v>
@@ -6443,21 +6381,21 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
-        <v>77</v>
+        <v>131</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G42" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H42" t="s" s="2">
         <v>77</v>
@@ -6469,16 +6407,16 @@
         <v>77</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>352</v>
+        <v>133</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>353</v>
+        <v>164</v>
       </c>
       <c r="N42" t="s" s="2">
-        <v>354</v>
+        <v>135</v>
       </c>
       <c r="O42" s="2"/>
       <c r="P42" t="s" s="2">
@@ -6504,13 +6442,13 @@
         <v>77</v>
       </c>
       <c r="X42" t="s" s="2">
-        <v>249</v>
+        <v>77</v>
       </c>
       <c r="Y42" t="s" s="2">
-        <v>355</v>
+        <v>77</v>
       </c>
       <c r="Z42" t="s" s="2">
-        <v>356</v>
+        <v>77</v>
       </c>
       <c r="AA42" t="s" s="2">
         <v>77</v>
@@ -6528,28 +6466,28 @@
         <v>77</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>351</v>
+        <v>167</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH42" t="s" s="2">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AI42" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AJ42" t="s" s="2">
-        <v>98</v>
+        <v>137</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>357</v>
+        <v>161</v>
       </c>
       <c r="AL42" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>358</v>
+        <v>77</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>77</v>
@@ -6557,45 +6495,45 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
-        <v>77</v>
+        <v>293</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G43" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H43" t="s" s="2">
         <v>77</v>
       </c>
       <c r="I43" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="J43" t="s" s="2">
         <v>87</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>360</v>
+        <v>132</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>361</v>
+        <v>294</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>362</v>
+        <v>295</v>
       </c>
       <c r="N43" t="s" s="2">
-        <v>363</v>
+        <v>135</v>
       </c>
       <c r="O43" t="s" s="2">
-        <v>364</v>
+        <v>141</v>
       </c>
       <c r="P43" t="s" s="2">
         <v>77</v>
@@ -6620,13 +6558,13 @@
         <v>77</v>
       </c>
       <c r="X43" t="s" s="2">
-        <v>187</v>
+        <v>77</v>
       </c>
       <c r="Y43" t="s" s="2">
-        <v>365</v>
+        <v>77</v>
       </c>
       <c r="Z43" t="s" s="2">
-        <v>366</v>
+        <v>77</v>
       </c>
       <c r="AA43" t="s" s="2">
         <v>77</v>
@@ -6644,28 +6582,28 @@
         <v>77</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>359</v>
+        <v>296</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH43" t="s" s="2">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AI43" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AJ43" t="s" s="2">
-        <v>98</v>
+        <v>137</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>77</v>
+        <v>129</v>
       </c>
       <c r="AL43" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>367</v>
+        <v>77</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>77</v>
@@ -6673,10 +6611,10 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>368</v>
+        <v>356</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>368</v>
+        <v>356</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -6687,7 +6625,7 @@
         <v>78</v>
       </c>
       <c r="G44" t="s" s="2">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="H44" t="s" s="2">
         <v>77</v>
@@ -6699,13 +6637,13 @@
         <v>77</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>304</v>
+        <v>157</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>369</v>
+        <v>357</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>370</v>
+        <v>358</v>
       </c>
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
@@ -6756,13 +6694,13 @@
         <v>77</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>368</v>
+        <v>356</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH44" t="s" s="2">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="AI44" t="s" s="2">
         <v>77</v>
@@ -6771,7 +6709,7 @@
         <v>98</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>371</v>
+        <v>359</v>
       </c>
       <c r="AL44" t="s" s="2">
         <v>77</v>
@@ -6785,10 +6723,10 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>372</v>
+        <v>360</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>372</v>
+        <v>360</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -6811,13 +6749,13 @@
         <v>77</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>157</v>
+        <v>182</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>158</v>
+        <v>361</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>159</v>
+        <v>362</v>
       </c>
       <c r="N45" s="2"/>
       <c r="O45" s="2"/>
@@ -6844,13 +6782,13 @@
         <v>77</v>
       </c>
       <c r="X45" t="s" s="2">
-        <v>77</v>
+        <v>249</v>
       </c>
       <c r="Y45" t="s" s="2">
-        <v>77</v>
+        <v>363</v>
       </c>
       <c r="Z45" t="s" s="2">
-        <v>77</v>
+        <v>364</v>
       </c>
       <c r="AA45" t="s" s="2">
         <v>77</v>
@@ -6868,7 +6806,7 @@
         <v>77</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>160</v>
+        <v>360</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>78</v>
@@ -6880,10 +6818,10 @@
         <v>77</v>
       </c>
       <c r="AJ45" t="s" s="2">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="AK45" t="s" s="2">
-        <v>161</v>
+        <v>252</v>
       </c>
       <c r="AL45" t="s" s="2">
         <v>77</v>
@@ -6897,14 +6835,14 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
-        <v>131</v>
+        <v>77</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" t="s" s="2">
@@ -6923,17 +6861,15 @@
         <v>77</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>132</v>
+        <v>366</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>133</v>
+        <v>367</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>164</v>
-      </c>
-      <c r="N46" t="s" s="2">
-        <v>135</v>
-      </c>
+        <v>368</v>
+      </c>
+      <c r="N46" s="2"/>
       <c r="O46" s="2"/>
       <c r="P46" t="s" s="2">
         <v>77</v>
@@ -6982,7 +6918,7 @@
         <v>77</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>167</v>
+        <v>365</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>78</v>
@@ -6994,16 +6930,16 @@
         <v>77</v>
       </c>
       <c r="AJ46" t="s" s="2">
-        <v>137</v>
+        <v>98</v>
       </c>
       <c r="AK46" t="s" s="2">
-        <v>161</v>
+        <v>369</v>
       </c>
       <c r="AL46" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>77</v>
+        <v>370</v>
       </c>
       <c r="AN46" t="s" s="2">
         <v>77</v>
@@ -7011,46 +6947,42 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
-        <v>312</v>
+        <v>77</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G47" t="s" s="2">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="H47" t="s" s="2">
         <v>77</v>
       </c>
       <c r="I47" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>132</v>
+        <v>305</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>313</v>
+        <v>372</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>314</v>
-      </c>
-      <c r="N47" t="s" s="2">
-        <v>135</v>
-      </c>
-      <c r="O47" t="s" s="2">
-        <v>141</v>
-      </c>
+        <v>373</v>
+      </c>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
       <c r="P47" t="s" s="2">
         <v>77</v>
       </c>
@@ -7098,22 +7030,22 @@
         <v>77</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>315</v>
+        <v>371</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH47" t="s" s="2">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="AI47" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AJ47" t="s" s="2">
-        <v>137</v>
+        <v>98</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>129</v>
+        <v>309</v>
       </c>
       <c r="AL47" t="s" s="2">
         <v>77</v>
@@ -7127,10 +7059,10 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -7141,7 +7073,7 @@
         <v>78</v>
       </c>
       <c r="G48" t="s" s="2">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="H48" t="s" s="2">
         <v>77</v>
@@ -7153,13 +7085,13 @@
         <v>77</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>157</v>
+        <v>285</v>
       </c>
       <c r="L48" t="s" s="2">
+        <v>375</v>
+      </c>
+      <c r="M48" t="s" s="2">
         <v>376</v>
-      </c>
-      <c r="M48" t="s" s="2">
-        <v>377</v>
       </c>
       <c r="N48" s="2"/>
       <c r="O48" s="2"/>
@@ -7210,13 +7142,13 @@
         <v>77</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH48" t="s" s="2">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AI48" t="s" s="2">
         <v>77</v>
@@ -7225,7 +7157,7 @@
         <v>98</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AL48" t="s" s="2">
         <v>77</v>
@@ -7239,10 +7171,10 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
@@ -7265,13 +7197,13 @@
         <v>77</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>182</v>
+        <v>157</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>380</v>
+        <v>158</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>381</v>
+        <v>159</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" s="2"/>
@@ -7298,13 +7230,13 @@
         <v>77</v>
       </c>
       <c r="X49" t="s" s="2">
-        <v>249</v>
+        <v>77</v>
       </c>
       <c r="Y49" t="s" s="2">
-        <v>382</v>
+        <v>77</v>
       </c>
       <c r="Z49" t="s" s="2">
-        <v>383</v>
+        <v>77</v>
       </c>
       <c r="AA49" t="s" s="2">
         <v>77</v>
@@ -7322,7 +7254,7 @@
         <v>77</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>379</v>
+        <v>160</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>78</v>
@@ -7334,10 +7266,10 @@
         <v>77</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>252</v>
+        <v>161</v>
       </c>
       <c r="AL49" t="s" s="2">
         <v>77</v>
@@ -7351,14 +7283,14 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
-        <v>77</v>
+        <v>131</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" t="s" s="2">
@@ -7377,15 +7309,17 @@
         <v>77</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>385</v>
+        <v>132</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>386</v>
+        <v>133</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>387</v>
-      </c>
-      <c r="N50" s="2"/>
+        <v>164</v>
+      </c>
+      <c r="N50" t="s" s="2">
+        <v>135</v>
+      </c>
       <c r="O50" s="2"/>
       <c r="P50" t="s" s="2">
         <v>77</v>
@@ -7434,7 +7368,7 @@
         <v>77</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>384</v>
+        <v>167</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>78</v>
@@ -7446,16 +7380,16 @@
         <v>77</v>
       </c>
       <c r="AJ50" t="s" s="2">
-        <v>98</v>
+        <v>137</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>388</v>
+        <v>161</v>
       </c>
       <c r="AL50" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>389</v>
+        <v>77</v>
       </c>
       <c r="AN50" t="s" s="2">
         <v>77</v>
@@ -7463,42 +7397,46 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
-        <v>77</v>
+        <v>293</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G51" t="s" s="2">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="H51" t="s" s="2">
         <v>77</v>
       </c>
       <c r="I51" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>324</v>
+        <v>132</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>391</v>
+        <v>294</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>392</v>
-      </c>
-      <c r="N51" s="2"/>
-      <c r="O51" s="2"/>
+        <v>295</v>
+      </c>
+      <c r="N51" t="s" s="2">
+        <v>135</v>
+      </c>
+      <c r="O51" t="s" s="2">
+        <v>141</v>
+      </c>
       <c r="P51" t="s" s="2">
         <v>77</v>
       </c>
@@ -7546,22 +7484,22 @@
         <v>77</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>390</v>
+        <v>296</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH51" t="s" s="2">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AI51" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AJ51" t="s" s="2">
-        <v>98</v>
+        <v>137</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>328</v>
+        <v>129</v>
       </c>
       <c r="AL51" t="s" s="2">
         <v>77</v>
@@ -7575,10 +7513,10 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>393</v>
+        <v>381</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>393</v>
+        <v>381</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
@@ -7589,7 +7527,7 @@
         <v>78</v>
       </c>
       <c r="G52" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H52" t="s" s="2">
         <v>77</v>
@@ -7598,16 +7536,16 @@
         <v>77</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>304</v>
+        <v>144</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>394</v>
+        <v>382</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>395</v>
+        <v>383</v>
       </c>
       <c r="N52" s="2"/>
       <c r="O52" s="2"/>
@@ -7658,7 +7596,7 @@
         <v>77</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>393</v>
+        <v>381</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>78</v>
@@ -7673,13 +7611,13 @@
         <v>98</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>396</v>
+        <v>149</v>
       </c>
       <c r="AL52" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>77</v>
+        <v>384</v>
       </c>
       <c r="AN52" t="s" s="2">
         <v>77</v>
@@ -7687,10 +7625,10 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>397</v>
+        <v>385</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>397</v>
+        <v>385</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
@@ -7716,10 +7654,10 @@
         <v>157</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>158</v>
+        <v>386</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>159</v>
+        <v>387</v>
       </c>
       <c r="N53" s="2"/>
       <c r="O53" s="2"/>
@@ -7770,7 +7708,7 @@
         <v>77</v>
       </c>
       <c r="AF53" t="s" s="2">
-        <v>160</v>
+        <v>385</v>
       </c>
       <c r="AG53" t="s" s="2">
         <v>78</v>
@@ -7782,10 +7720,10 @@
         <v>77</v>
       </c>
       <c r="AJ53" t="s" s="2">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>161</v>
+        <v>388</v>
       </c>
       <c r="AL53" t="s" s="2">
         <v>77</v>
@@ -7799,21 +7737,21 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>398</v>
+        <v>389</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>398</v>
+        <v>389</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" t="s" s="2">
-        <v>131</v>
+        <v>77</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G54" t="s" s="2">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="H54" t="s" s="2">
         <v>77</v>
@@ -7825,17 +7763,15 @@
         <v>77</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>132</v>
+        <v>182</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>133</v>
+        <v>390</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>164</v>
-      </c>
-      <c r="N54" t="s" s="2">
-        <v>135</v>
-      </c>
+        <v>391</v>
+      </c>
+      <c r="N54" s="2"/>
       <c r="O54" s="2"/>
       <c r="P54" t="s" s="2">
         <v>77</v>
@@ -7860,13 +7796,13 @@
         <v>77</v>
       </c>
       <c r="X54" t="s" s="2">
-        <v>77</v>
+        <v>249</v>
       </c>
       <c r="Y54" t="s" s="2">
-        <v>77</v>
+        <v>392</v>
       </c>
       <c r="Z54" t="s" s="2">
-        <v>77</v>
+        <v>393</v>
       </c>
       <c r="AA54" t="s" s="2">
         <v>77</v>
@@ -7884,28 +7820,28 @@
         <v>77</v>
       </c>
       <c r="AF54" t="s" s="2">
-        <v>167</v>
+        <v>389</v>
       </c>
       <c r="AG54" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH54" t="s" s="2">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="AI54" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AJ54" t="s" s="2">
-        <v>137</v>
+        <v>98</v>
       </c>
       <c r="AK54" t="s" s="2">
-        <v>161</v>
+        <v>252</v>
       </c>
       <c r="AL54" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>77</v>
+        <v>394</v>
       </c>
       <c r="AN54" t="s" s="2">
         <v>77</v>
@@ -7913,46 +7849,42 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" t="s" s="2">
-        <v>312</v>
+        <v>77</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G55" t="s" s="2">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="H55" t="s" s="2">
         <v>77</v>
       </c>
       <c r="I55" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="J55" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>132</v>
+        <v>320</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>313</v>
+        <v>396</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>314</v>
-      </c>
-      <c r="N55" t="s" s="2">
-        <v>135</v>
-      </c>
-      <c r="O55" t="s" s="2">
-        <v>141</v>
-      </c>
+        <v>397</v>
+      </c>
+      <c r="N55" s="2"/>
+      <c r="O55" s="2"/>
       <c r="P55" t="s" s="2">
         <v>77</v>
       </c>
@@ -8000,28 +7932,28 @@
         <v>77</v>
       </c>
       <c r="AF55" t="s" s="2">
-        <v>315</v>
+        <v>395</v>
       </c>
       <c r="AG55" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH55" t="s" s="2">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="AI55" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AJ55" t="s" s="2">
-        <v>137</v>
+        <v>98</v>
       </c>
       <c r="AK55" t="s" s="2">
-        <v>129</v>
+        <v>398</v>
       </c>
       <c r="AL55" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AM55" t="s" s="2">
-        <v>77</v>
+        <v>399</v>
       </c>
       <c r="AN55" t="s" s="2">
         <v>77</v>
@@ -8043,7 +7975,7 @@
         <v>78</v>
       </c>
       <c r="G56" t="s" s="2">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="H56" t="s" s="2">
         <v>77</v>
@@ -8052,10 +7984,10 @@
         <v>77</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>144</v>
+        <v>320</v>
       </c>
       <c r="L56" t="s" s="2">
         <v>401</v>
@@ -8118,7 +8050,7 @@
         <v>78</v>
       </c>
       <c r="AH56" t="s" s="2">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="AI56" t="s" s="2">
         <v>77</v>
@@ -8127,13 +8059,13 @@
         <v>98</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>149</v>
+        <v>403</v>
       </c>
       <c r="AL56" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AM56" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="AN56" t="s" s="2">
         <v>77</v>
@@ -8141,10 +8073,10 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" t="s" s="2">
@@ -8167,13 +8099,13 @@
         <v>77</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>157</v>
+        <v>406</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="N57" s="2"/>
       <c r="O57" s="2"/>
@@ -8200,13 +8132,13 @@
         <v>77</v>
       </c>
       <c r="X57" t="s" s="2">
-        <v>77</v>
+        <v>249</v>
       </c>
       <c r="Y57" t="s" s="2">
-        <v>77</v>
+        <v>409</v>
       </c>
       <c r="Z57" t="s" s="2">
-        <v>77</v>
+        <v>410</v>
       </c>
       <c r="AA57" t="s" s="2">
         <v>77</v>
@@ -8224,7 +8156,7 @@
         <v>77</v>
       </c>
       <c r="AF57" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="AG57" t="s" s="2">
         <v>78</v>
@@ -8239,13 +8171,13 @@
         <v>98</v>
       </c>
       <c r="AK57" t="s" s="2">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="AL57" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AM57" t="s" s="2">
-        <v>77</v>
+        <v>412</v>
       </c>
       <c r="AN57" t="s" s="2">
         <v>77</v>
@@ -8253,10 +8185,10 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>408</v>
+        <v>413</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>408</v>
+        <v>413</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" t="s" s="2">
@@ -8267,7 +8199,7 @@
         <v>78</v>
       </c>
       <c r="G58" t="s" s="2">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="H58" t="s" s="2">
         <v>77</v>
@@ -8276,19 +8208,23 @@
         <v>77</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="K58" t="s" s="2">
         <v>182</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>409</v>
+        <v>414</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>410</v>
-      </c>
-      <c r="N58" s="2"/>
-      <c r="O58" s="2"/>
+        <v>415</v>
+      </c>
+      <c r="N58" t="s" s="2">
+        <v>416</v>
+      </c>
+      <c r="O58" t="s" s="2">
+        <v>417</v>
+      </c>
       <c r="P58" t="s" s="2">
         <v>77</v>
       </c>
@@ -8312,13 +8248,13 @@
         <v>77</v>
       </c>
       <c r="X58" t="s" s="2">
-        <v>249</v>
+        <v>187</v>
       </c>
       <c r="Y58" t="s" s="2">
-        <v>411</v>
+        <v>418</v>
       </c>
       <c r="Z58" t="s" s="2">
-        <v>412</v>
+        <v>419</v>
       </c>
       <c r="AA58" t="s" s="2">
         <v>77</v>
@@ -8336,13 +8272,13 @@
         <v>77</v>
       </c>
       <c r="AF58" t="s" s="2">
-        <v>408</v>
+        <v>413</v>
       </c>
       <c r="AG58" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH58" t="s" s="2">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AI58" t="s" s="2">
         <v>77</v>
@@ -8351,13 +8287,13 @@
         <v>98</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>252</v>
+        <v>77</v>
       </c>
       <c r="AL58" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AM58" t="s" s="2">
-        <v>413</v>
+        <v>420</v>
       </c>
       <c r="AN58" t="s" s="2">
         <v>77</v>
@@ -8365,10 +8301,10 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>414</v>
+        <v>421</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>414</v>
+        <v>421</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s" s="2">
@@ -8379,7 +8315,7 @@
         <v>78</v>
       </c>
       <c r="G59" t="s" s="2">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="H59" t="s" s="2">
         <v>77</v>
@@ -8391,13 +8327,13 @@
         <v>77</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>339</v>
+        <v>422</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>415</v>
+        <v>50</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="N59" s="2"/>
       <c r="O59" s="2"/>
@@ -8448,13 +8384,13 @@
         <v>77</v>
       </c>
       <c r="AF59" t="s" s="2">
-        <v>414</v>
+        <v>421</v>
       </c>
       <c r="AG59" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH59" t="s" s="2">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AI59" t="s" s="2">
         <v>77</v>
@@ -8463,472 +8399,20 @@
         <v>98</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>417</v>
+        <v>424</v>
       </c>
       <c r="AL59" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AM59" t="s" s="2">
-        <v>418</v>
+        <v>425</v>
       </c>
       <c r="AN59" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="60" hidden="true">
-      <c r="A60" t="s" s="2">
-        <v>419</v>
-      </c>
-      <c r="B60" t="s" s="2">
-        <v>419</v>
-      </c>
-      <c r="C60" s="2"/>
-      <c r="D60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="E60" s="2"/>
-      <c r="F60" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G60" t="s" s="2">
-        <v>86</v>
-      </c>
-      <c r="H60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="J60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="K60" t="s" s="2">
-        <v>339</v>
-      </c>
-      <c r="L60" t="s" s="2">
-        <v>420</v>
-      </c>
-      <c r="M60" t="s" s="2">
-        <v>421</v>
-      </c>
-      <c r="N60" s="2"/>
-      <c r="O60" s="2"/>
-      <c r="P60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Q60" s="2"/>
-      <c r="R60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="S60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="T60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="U60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="V60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="W60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="X60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Y60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Z60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AA60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AB60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AE60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF60" t="s" s="2">
-        <v>419</v>
-      </c>
-      <c r="AG60" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH60" t="s" s="2">
-        <v>86</v>
-      </c>
-      <c r="AI60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AJ60" t="s" s="2">
-        <v>98</v>
-      </c>
-      <c r="AK60" t="s" s="2">
-        <v>422</v>
-      </c>
-      <c r="AL60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM60" t="s" s="2">
-        <v>423</v>
-      </c>
-      <c r="AN60" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="61" hidden="true">
-      <c r="A61" t="s" s="2">
-        <v>424</v>
-      </c>
-      <c r="B61" t="s" s="2">
-        <v>424</v>
-      </c>
-      <c r="C61" s="2"/>
-      <c r="D61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="E61" s="2"/>
-      <c r="F61" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G61" t="s" s="2">
-        <v>86</v>
-      </c>
-      <c r="H61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="J61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="K61" t="s" s="2">
-        <v>425</v>
-      </c>
-      <c r="L61" t="s" s="2">
-        <v>426</v>
-      </c>
-      <c r="M61" t="s" s="2">
-        <v>427</v>
-      </c>
-      <c r="N61" s="2"/>
-      <c r="O61" s="2"/>
-      <c r="P61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Q61" s="2"/>
-      <c r="R61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="S61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="T61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="U61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="V61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="W61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="X61" t="s" s="2">
-        <v>249</v>
-      </c>
-      <c r="Y61" t="s" s="2">
-        <v>428</v>
-      </c>
-      <c r="Z61" t="s" s="2">
-        <v>429</v>
-      </c>
-      <c r="AA61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AB61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AE61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF61" t="s" s="2">
-        <v>424</v>
-      </c>
-      <c r="AG61" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH61" t="s" s="2">
-        <v>86</v>
-      </c>
-      <c r="AI61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AJ61" t="s" s="2">
-        <v>98</v>
-      </c>
-      <c r="AK61" t="s" s="2">
-        <v>430</v>
-      </c>
-      <c r="AL61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM61" t="s" s="2">
-        <v>431</v>
-      </c>
-      <c r="AN61" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="62" hidden="true">
-      <c r="A62" t="s" s="2">
-        <v>432</v>
-      </c>
-      <c r="B62" t="s" s="2">
-        <v>432</v>
-      </c>
-      <c r="C62" s="2"/>
-      <c r="D62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="E62" s="2"/>
-      <c r="F62" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G62" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="H62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="J62" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="K62" t="s" s="2">
-        <v>182</v>
-      </c>
-      <c r="L62" t="s" s="2">
-        <v>433</v>
-      </c>
-      <c r="M62" t="s" s="2">
-        <v>434</v>
-      </c>
-      <c r="N62" t="s" s="2">
-        <v>435</v>
-      </c>
-      <c r="O62" t="s" s="2">
-        <v>436</v>
-      </c>
-      <c r="P62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Q62" s="2"/>
-      <c r="R62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="S62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="T62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="U62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="V62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="W62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="X62" t="s" s="2">
-        <v>187</v>
-      </c>
-      <c r="Y62" t="s" s="2">
-        <v>437</v>
-      </c>
-      <c r="Z62" t="s" s="2">
-        <v>438</v>
-      </c>
-      <c r="AA62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AB62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AE62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF62" t="s" s="2">
-        <v>432</v>
-      </c>
-      <c r="AG62" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH62" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AI62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AJ62" t="s" s="2">
-        <v>98</v>
-      </c>
-      <c r="AK62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AL62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM62" t="s" s="2">
-        <v>439</v>
-      </c>
-      <c r="AN62" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="63" hidden="true">
-      <c r="A63" t="s" s="2">
-        <v>440</v>
-      </c>
-      <c r="B63" t="s" s="2">
-        <v>440</v>
-      </c>
-      <c r="C63" s="2"/>
-      <c r="D63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="E63" s="2"/>
-      <c r="F63" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G63" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="H63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="J63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="K63" t="s" s="2">
-        <v>441</v>
-      </c>
-      <c r="L63" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="M63" t="s" s="2">
-        <v>442</v>
-      </c>
-      <c r="N63" s="2"/>
-      <c r="O63" s="2"/>
-      <c r="P63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Q63" s="2"/>
-      <c r="R63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="S63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="T63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="U63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="V63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="W63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="X63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Y63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Z63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AA63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AB63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AE63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF63" t="s" s="2">
-        <v>440</v>
-      </c>
-      <c r="AG63" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH63" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AI63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AJ63" t="s" s="2">
-        <v>98</v>
-      </c>
-      <c r="AK63" t="s" s="2">
-        <v>443</v>
-      </c>
-      <c r="AL63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM63" t="s" s="2">
-        <v>444</v>
-      </c>
-      <c r="AN63" t="s" s="2">
         <v>77</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AN63">
+  <autoFilter ref="A1:AN59">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -8938,7 +8422,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI62">
+  <conditionalFormatting sqref="A2:AI58">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
change CBC to just CH and add an example of allergy
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-VA.MHV.PHR.LabSpecimen.xlsx
+++ b/docs/StructureDefinition-VA.MHV.PHR.LabSpecimen.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.8-beta</t>
+    <t>0.1.9-beta</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-04-12T10:49:54-05:00</t>
+    <t>2023-04-14T09:56:36-05:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
updates of CH, with addition of Ken's example
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-VA.MHV.PHR.LabSpecimen.xlsx
+++ b/docs/StructureDefinition-VA.MHV.PHR.LabSpecimen.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.9-beta</t>
+    <t>0.1.10-beta</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-04-14T09:56:36-05:00</t>
+    <t>2023-04-17T18:54:15-05:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
CH allow valueString as well as valueQuantity
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-VA.MHV.PHR.LabSpecimen.xlsx
+++ b/docs/StructureDefinition-VA.MHV.PHR.LabSpecimen.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.10-beta</t>
+    <t>0.1.11-beta</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-04-17T19:11:15-05:00</t>
+    <t>2023-04-24T08:03:17-05:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
add Panel to ch, some fixes to allergy
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-VA.MHV.PHR.LabSpecimen.xlsx
+++ b/docs/StructureDefinition-VA.MHV.PHR.LabSpecimen.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.11-beta</t>
+    <t>0.1.12-beta</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-04-24T08:03:17-05:00</t>
+    <t>2023-05-01T08:16:19-05:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
complete allergy examples. Allergy: add two new map elements, and eliminate an invalid map.
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-VA.MHV.PHR.LabSpecimen.xlsx
+++ b/docs/StructureDefinition-VA.MHV.PHR.LabSpecimen.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.12-beta</t>
+    <t>0.1.13-beta</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-05-01T08:16:19-05:00</t>
+    <t>2023-05-02T08:13:48-05:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
Add examples for allergy and chem-hem
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-VA.MHV.PHR.LabSpecimen.xlsx
+++ b/docs/StructureDefinition-VA.MHV.PHR.LabSpecimen.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.13-beta</t>
+    <t>0.1.14-beta</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-05-02T08:13:48-05:00</t>
+    <t>2023-05-04T14:24:58-05:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
added a section on use of the MHV FHIR API as a different perspective added business rule exceptions such as not translating allergy notes Updated Discharge Summary note as we do not get an id value from the ADT
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-VA.MHV.PHR.LabSpecimen.xlsx
+++ b/docs/StructureDefinition-VA.MHV.PHR.LabSpecimen.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.14-beta</t>
+    <t>0.1.15-beta</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-05-04T14:24:58-05:00</t>
+    <t>2023-06-07T11:47:17-05:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
add first draft of medication. Few other updates.
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-VA.MHV.PHR.LabSpecimen.xlsx
+++ b/docs/StructureDefinition-VA.MHV.PHR.LabSpecimen.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.16-beta</t>
+    <t>0.1.17-beta</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-06-16T14:48:21-05:00</t>
+    <t>2023-07-13T09:22:36-05:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
notes on allergies, updates to medications analysis
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-VA.MHV.PHR.LabSpecimen.xlsx
+++ b/docs/StructureDefinition-VA.MHV.PHR.LabSpecimen.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.17-beta</t>
+    <t>0.1.18-beta</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-07-13T09:22:36-05:00</t>
+    <t>2023-07-19T13:17:04-05:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
fill gaps in allergies, and immunizations. Add code review on vital-signs.
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-VA.MHV.PHR.LabSpecimen.xlsx
+++ b/docs/StructureDefinition-VA.MHV.PHR.LabSpecimen.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.19-beta</t>
+    <t>0.1.20-beta</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-08-18T07:55:35-05:00</t>
+    <t>2023-08-22T11:16:10-05:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
change to contained for Organization, Location, and Practitioner clarify turning on HAPI resource validation add more detail on proper handling of source id
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-VA.MHV.PHR.LabSpecimen.xlsx
+++ b/docs/StructureDefinition-VA.MHV.PHR.LabSpecimen.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2105" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2105" uniqueCount="388">
   <si>
     <t>Property</t>
   </si>
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.2.0</t>
+    <t>0.2.1</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-08-22T16:36:15-05:00</t>
+    <t>2023-08-24T09:48:15-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -158,6 +158,10 @@
   </si>
   <si>
     <t>A sample to be used for analysis.</t>
+  </si>
+  <si>
+    <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
+dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}</t>
   </si>
   <si>
     <t>Role[classCode=SPEC]</t>
@@ -1700,10 +1704,10 @@
         <v>37</v>
       </c>
       <c r="AJ1" t="s" s="2">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="AK1" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AL1" t="s" s="2">
         <v>37</v>
@@ -1712,15 +1716,15 @@
         <v>37</v>
       </c>
       <c r="AN1" t="s" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" hidden="true">
       <c r="A2" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" t="s" s="2">
@@ -1731,7 +1735,7 @@
         <v>38</v>
       </c>
       <c r="G2" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H2" t="s" s="2">
         <v>37</v>
@@ -1740,19 +1744,19 @@
         <v>37</v>
       </c>
       <c r="J2" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K2" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L2" t="s" s="2">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M2" t="s" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N2" t="s" s="2">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="O2" s="2"/>
       <c r="P2" t="s" s="2">
@@ -1802,13 +1806,13 @@
         <v>37</v>
       </c>
       <c r="AF2" t="s" s="2">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AG2" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH2" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI2" t="s" s="2">
         <v>37</v>
@@ -1831,10 +1835,10 @@
     </row>
     <row r="3" hidden="true">
       <c r="A3" t="s" s="2">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" t="s" s="2">
@@ -1845,7 +1849,7 @@
         <v>38</v>
       </c>
       <c r="G3" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H3" t="s" s="2">
         <v>37</v>
@@ -1854,16 +1858,16 @@
         <v>37</v>
       </c>
       <c r="J3" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K3" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L3" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M3" t="s" s="2">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
@@ -1914,19 +1918,19 @@
         <v>37</v>
       </c>
       <c r="AF3" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AG3" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH3" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI3" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ3" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK3" t="s" s="2">
         <v>37</v>
@@ -1943,10 +1947,10 @@
     </row>
     <row r="4" hidden="true">
       <c r="A4" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" t="s" s="2">
@@ -1957,28 +1961,28 @@
         <v>38</v>
       </c>
       <c r="G4" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H4" t="s" s="2">
         <v>37</v>
       </c>
       <c r="I4" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J4" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K4" t="s" s="2">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M4" t="s" s="2">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N4" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O4" s="2"/>
       <c r="P4" t="s" s="2">
@@ -2028,19 +2032,19 @@
         <v>37</v>
       </c>
       <c r="AF4" t="s" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AG4" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH4" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI4" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ4" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK4" t="s" s="2">
         <v>37</v>
@@ -2057,10 +2061,10 @@
     </row>
     <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" t="s" s="2">
@@ -2071,7 +2075,7 @@
         <v>38</v>
       </c>
       <c r="G5" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H5" t="s" s="2">
         <v>37</v>
@@ -2083,16 +2087,16 @@
         <v>37</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M5" t="s" s="2">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N5" t="s" s="2">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="O5" s="2"/>
       <c r="P5" t="s" s="2">
@@ -2118,13 +2122,13 @@
         <v>37</v>
       </c>
       <c r="X5" t="s" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="Y5" t="s" s="2">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="Z5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AA5" t="s" s="2">
         <v>37</v>
@@ -2142,19 +2146,19 @@
         <v>37</v>
       </c>
       <c r="AF5" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AG5" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH5" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI5" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ5" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK5" t="s" s="2">
         <v>37</v>
@@ -2171,21 +2175,21 @@
     </row>
     <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" t="s" s="2">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" t="s" s="2">
         <v>38</v>
       </c>
       <c r="G6" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H6" t="s" s="2">
         <v>37</v>
@@ -2197,16 +2201,16 @@
         <v>37</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M6" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="N6" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="O6" s="2"/>
       <c r="P6" t="s" s="2">
@@ -2256,22 +2260,22 @@
         <v>37</v>
       </c>
       <c r="AF6" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AG6" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH6" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI6" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ6" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK6" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AL6" t="s" s="2">
         <v>37</v>
@@ -2285,14 +2289,14 @@
     </row>
     <row r="7" hidden="true">
       <c r="A7" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" t="s" s="2">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" t="s" s="2">
@@ -2311,16 +2315,16 @@
         <v>37</v>
       </c>
       <c r="K7" t="s" s="2">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L7" t="s" s="2">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="M7" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="N7" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="O7" s="2"/>
       <c r="P7" t="s" s="2">
@@ -2370,7 +2374,7 @@
         <v>37</v>
       </c>
       <c r="AF7" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AG7" t="s" s="2">
         <v>38</v>
@@ -2385,7 +2389,7 @@
         <v>37</v>
       </c>
       <c r="AK7" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AL7" t="s" s="2">
         <v>37</v>
@@ -2399,14 +2403,14 @@
     </row>
     <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" t="s" s="2">
@@ -2425,16 +2429,16 @@
         <v>37</v>
       </c>
       <c r="K8" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L8" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M8" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N8" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O8" s="2"/>
       <c r="P8" t="s" s="2">
@@ -2484,7 +2488,7 @@
         <v>37</v>
       </c>
       <c r="AF8" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AG8" t="s" s="2">
         <v>38</v>
@@ -2496,10 +2500,10 @@
         <v>37</v>
       </c>
       <c r="AJ8" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AK8" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AL8" t="s" s="2">
         <v>37</v>
@@ -2513,14 +2517,14 @@
     </row>
     <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" t="s" s="2">
@@ -2533,25 +2537,25 @@
         <v>37</v>
       </c>
       <c r="I9" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J9" t="s" s="2">
         <v>37</v>
       </c>
       <c r="K9" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L9" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="M9" t="s" s="2">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="N9" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O9" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="P9" t="s" s="2">
         <v>37</v>
@@ -2600,7 +2604,7 @@
         <v>37</v>
       </c>
       <c r="AF9" t="s" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AG9" t="s" s="2">
         <v>38</v>
@@ -2612,10 +2616,10 @@
         <v>37</v>
       </c>
       <c r="AJ9" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AK9" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AL9" t="s" s="2">
         <v>37</v>
@@ -2629,10 +2633,10 @@
     </row>
     <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" t="s" s="2">
@@ -2640,7 +2644,7 @@
       </c>
       <c r="E10" s="2"/>
       <c r="F10" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G10" t="s" s="2">
         <v>39</v>
@@ -2652,16 +2656,16 @@
         <v>37</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="M10" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
@@ -2700,17 +2704,17 @@
         <v>37</v>
       </c>
       <c r="AB10" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AC10" s="2"/>
       <c r="AD10" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AE10" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="AF10" t="s" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AG10" t="s" s="2">
         <v>38</v>
@@ -2722,40 +2726,40 @@
         <v>37</v>
       </c>
       <c r="AJ10" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK10" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="AL10" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="AM10" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="AN10" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C11" t="s" s="2">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D11" t="s" s="2">
         <v>37</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G11" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H11" t="s" s="2">
         <v>37</v>
@@ -2764,16 +2768,16 @@
         <v>37</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="M11" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
@@ -2824,7 +2828,7 @@
         <v>37</v>
       </c>
       <c r="AF11" t="s" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AG11" t="s" s="2">
         <v>38</v>
@@ -2836,16 +2840,16 @@
         <v>37</v>
       </c>
       <c r="AJ11" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK11" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="AL11" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="AM11" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="AN11" t="s" s="2">
         <v>37</v>
@@ -2853,10 +2857,10 @@
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" t="s" s="2">
@@ -2867,7 +2871,7 @@
         <v>38</v>
       </c>
       <c r="G12" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H12" t="s" s="2">
         <v>37</v>
@@ -2879,13 +2883,13 @@
         <v>37</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="M12" t="s" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
@@ -2936,13 +2940,13 @@
         <v>37</v>
       </c>
       <c r="AF12" t="s" s="2">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AG12" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH12" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI12" t="s" s="2">
         <v>37</v>
@@ -2951,7 +2955,7 @@
         <v>37</v>
       </c>
       <c r="AK12" t="s" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AL12" t="s" s="2">
         <v>37</v>
@@ -2965,14 +2969,14 @@
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" t="s" s="2">
@@ -2991,16 +2995,16 @@
         <v>37</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M13" t="s" s="2">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="N13" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O13" s="2"/>
       <c r="P13" t="s" s="2">
@@ -3038,19 +3042,19 @@
         <v>37</v>
       </c>
       <c r="AB13" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AC13" t="s" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AD13" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="AF13" t="s" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AG13" t="s" s="2">
         <v>38</v>
@@ -3062,10 +3066,10 @@
         <v>37</v>
       </c>
       <c r="AJ13" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AK13" t="s" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AL13" t="s" s="2">
         <v>37</v>
@@ -3079,10 +3083,10 @@
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" t="s" s="2">
@@ -3090,34 +3094,34 @@
       </c>
       <c r="E14" s="2"/>
       <c r="F14" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G14" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H14" t="s" s="2">
         <v>37</v>
       </c>
       <c r="I14" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="N14" t="s" s="2">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="O14" t="s" s="2">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="P14" t="s" s="2">
         <v>37</v>
@@ -3127,7 +3131,7 @@
         <v>37</v>
       </c>
       <c r="S14" t="s" s="2">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="T14" t="s" s="2">
         <v>37</v>
@@ -3142,13 +3146,13 @@
         <v>37</v>
       </c>
       <c r="X14" t="s" s="2">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="Y14" t="s" s="2">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="Z14" t="s" s="2">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="AA14" t="s" s="2">
         <v>37</v>
@@ -3166,28 +3170,28 @@
         <v>37</v>
       </c>
       <c r="AF14" t="s" s="2">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="AG14" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH14" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI14" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="AL14" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM14" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AN14" t="s" s="2">
         <v>37</v>
@@ -3195,10 +3199,10 @@
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" t="s" s="2">
@@ -3209,7 +3213,7 @@
         <v>38</v>
       </c>
       <c r="G15" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H15" t="s" s="2">
         <v>37</v>
@@ -3218,22 +3222,22 @@
         <v>37</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="N15" t="s" s="2">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="O15" t="s" s="2">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="P15" t="s" s="2">
         <v>37</v>
@@ -3258,13 +3262,13 @@
         <v>37</v>
       </c>
       <c r="X15" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="Y15" t="s" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="Z15" t="s" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AA15" t="s" s="2">
         <v>37</v>
@@ -3282,28 +3286,28 @@
         <v>37</v>
       </c>
       <c r="AF15" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="AG15" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH15" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI15" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="AL15" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM15" t="s" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="AN15" t="s" s="2">
         <v>37</v>
@@ -3311,10 +3315,10 @@
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" t="s" s="2">
@@ -3325,7 +3329,7 @@
         <v>38</v>
       </c>
       <c r="G16" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H16" t="s" s="2">
         <v>37</v>
@@ -3334,22 +3338,22 @@
         <v>37</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="N16" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="O16" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="P16" t="s" s="2">
         <v>37</v>
@@ -3362,7 +3366,7 @@
         <v>37</v>
       </c>
       <c r="T16" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="U16" t="s" s="2">
         <v>37</v>
@@ -3398,28 +3402,28 @@
         <v>37</v>
       </c>
       <c r="AF16" t="s" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="AG16" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH16" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI16" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AL16" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM16" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="AN16" t="s" s="2">
         <v>37</v>
@@ -3427,10 +3431,10 @@
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" t="s" s="2">
@@ -3441,7 +3445,7 @@
         <v>38</v>
       </c>
       <c r="G17" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H17" t="s" s="2">
         <v>37</v>
@@ -3450,19 +3454,19 @@
         <v>37</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="N17" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="O17" s="2"/>
       <c r="P17" t="s" s="2">
@@ -3476,7 +3480,7 @@
         <v>37</v>
       </c>
       <c r="T17" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="U17" t="s" s="2">
         <v>37</v>
@@ -3512,28 +3516,28 @@
         <v>37</v>
       </c>
       <c r="AF17" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="AG17" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH17" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI17" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="AL17" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM17" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="AN17" t="s" s="2">
         <v>37</v>
@@ -3541,10 +3545,10 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s" s="2">
@@ -3555,7 +3559,7 @@
         <v>38</v>
       </c>
       <c r="G18" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H18" t="s" s="2">
         <v>37</v>
@@ -3564,16 +3568,16 @@
         <v>37</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
@@ -3624,28 +3628,28 @@
         <v>37</v>
       </c>
       <c r="AF18" t="s" s="2">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="AG18" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH18" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI18" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK18" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="AL18" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="AN18" t="s" s="2">
         <v>37</v>
@@ -3653,10 +3657,10 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s" s="2">
@@ -3667,7 +3671,7 @@
         <v>38</v>
       </c>
       <c r="G19" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H19" t="s" s="2">
         <v>37</v>
@@ -3676,19 +3680,19 @@
         <v>37</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="N19" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="O19" s="2"/>
       <c r="P19" t="s" s="2">
@@ -3738,28 +3742,28 @@
         <v>37</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AG19" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH19" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI19" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="AL19" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AN19" t="s" s="2">
         <v>37</v>
@@ -3767,10 +3771,10 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s" s="2">
@@ -3781,7 +3785,7 @@
         <v>38</v>
       </c>
       <c r="G20" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H20" t="s" s="2">
         <v>37</v>
@@ -3790,16 +3794,16 @@
         <v>37</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
@@ -3850,39 +3854,39 @@
         <v>37</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AG20" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH20" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI20" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="AN20" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s" s="2">
@@ -3893,28 +3897,28 @@
         <v>38</v>
       </c>
       <c r="G21" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H21" t="s" s="2">
         <v>37</v>
       </c>
       <c r="I21" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="N21" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="O21" s="2"/>
       <c r="P21" t="s" s="2">
@@ -3940,13 +3944,13 @@
         <v>37</v>
       </c>
       <c r="X21" t="s" s="2">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="Y21" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="Z21" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="AA21" t="s" s="2">
         <v>37</v>
@@ -3964,39 +3968,39 @@
         <v>37</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH21" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI21" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="AN21" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
@@ -4004,31 +4008,31 @@
       </c>
       <c r="E22" s="2"/>
       <c r="F22" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G22" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H22" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I22" t="s" s="2">
         <v>37</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="N22" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="O22" s="2"/>
       <c r="P22" t="s" s="2">
@@ -4054,13 +4058,13 @@
         <v>37</v>
       </c>
       <c r="X22" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="Y22" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="Z22" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="AA22" t="s" s="2">
         <v>37</v>
@@ -4078,39 +4082,39 @@
         <v>37</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH22" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI22" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="AN22" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
@@ -4130,20 +4134,20 @@
         <v>37</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="P23" t="s" s="2">
         <v>37</v>
@@ -4192,25 +4196,25 @@
         <v>37</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH23" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI23" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="AM23" t="s" s="2">
         <v>37</v>
@@ -4221,10 +4225,10 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
@@ -4244,16 +4248,16 @@
         <v>37</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
@@ -4304,28 +4308,28 @@
         <v>37</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH24" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI24" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="AN24" t="s" s="2">
         <v>37</v>
@@ -4333,10 +4337,10 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
@@ -4359,16 +4363,16 @@
         <v>37</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="O25" s="2"/>
       <c r="P25" t="s" s="2">
@@ -4418,7 +4422,7 @@
         <v>37</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>38</v>
@@ -4430,10 +4434,10 @@
         <v>37</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="AL25" t="s" s="2">
         <v>37</v>
@@ -4447,10 +4451,10 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
@@ -4473,16 +4477,16 @@
         <v>37</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="N26" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="O26" s="2"/>
       <c r="P26" t="s" s="2">
@@ -4532,7 +4536,7 @@
         <v>37</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>38</v>
@@ -4544,16 +4548,16 @@
         <v>37</v>
       </c>
       <c r="AJ26" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="AN26" t="s" s="2">
         <v>37</v>
@@ -4561,10 +4565,10 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
@@ -4575,10 +4579,10 @@
         <v>38</v>
       </c>
       <c r="G27" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H27" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I27" t="s" s="2">
         <v>37</v>
@@ -4587,13 +4591,13 @@
         <v>37</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
@@ -4644,28 +4648,28 @@
         <v>37</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH27" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI27" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ27" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AL27" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN27" t="s" s="2">
         <v>37</v>
@@ -4673,10 +4677,10 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
@@ -4687,7 +4691,7 @@
         <v>38</v>
       </c>
       <c r="G28" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H28" t="s" s="2">
         <v>37</v>
@@ -4699,13 +4703,13 @@
         <v>37</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
@@ -4756,13 +4760,13 @@
         <v>37</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH28" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI28" t="s" s="2">
         <v>37</v>
@@ -4771,7 +4775,7 @@
         <v>37</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AL28" t="s" s="2">
         <v>37</v>
@@ -4785,14 +4789,14 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" t="s" s="2">
@@ -4811,16 +4815,16 @@
         <v>37</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="N29" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O29" s="2"/>
       <c r="P29" t="s" s="2">
@@ -4870,7 +4874,7 @@
         <v>37</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>38</v>
@@ -4882,10 +4886,10 @@
         <v>37</v>
       </c>
       <c r="AJ29" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AL29" t="s" s="2">
         <v>37</v>
@@ -4899,14 +4903,14 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" t="s" s="2">
@@ -4919,25 +4923,25 @@
         <v>37</v>
       </c>
       <c r="I30" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="N30" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O30" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="P30" t="s" s="2">
         <v>37</v>
@@ -4986,7 +4990,7 @@
         <v>37</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>38</v>
@@ -4998,10 +5002,10 @@
         <v>37</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AL30" t="s" s="2">
         <v>37</v>
@@ -5015,10 +5019,10 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -5038,16 +5042,16 @@
         <v>37</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
@@ -5098,28 +5102,28 @@
         <v>37</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH31" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI31" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>37</v>
@@ -5127,10 +5131,10 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -5141,7 +5145,7 @@
         <v>38</v>
       </c>
       <c r="G32" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H32" t="s" s="2">
         <v>37</v>
@@ -5150,16 +5154,16 @@
         <v>37</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
@@ -5198,38 +5202,38 @@
         <v>37</v>
       </c>
       <c r="AB32" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="AC32" s="2"/>
       <c r="AD32" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH32" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI32" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>37</v>
@@ -5237,13 +5241,13 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C33" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D33" t="s" s="2">
         <v>37</v>
@@ -5253,25 +5257,25 @@
         <v>38</v>
       </c>
       <c r="G33" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H33" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I33" t="s" s="2">
         <v>37</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
@@ -5322,39 +5326,39 @@
         <v>37</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH33" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI33" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="AN33" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -5374,16 +5378,16 @@
         <v>37</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
@@ -5434,25 +5438,25 @@
         <v>37</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH34" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI34" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK34" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="AM34" t="s" s="2">
         <v>37</v>
@@ -5463,10 +5467,10 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
@@ -5489,13 +5493,13 @@
         <v>37</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
@@ -5546,28 +5550,28 @@
         <v>37</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH35" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI35" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="AL35" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="AN35" t="s" s="2">
         <v>37</v>
@@ -5575,10 +5579,10 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -5601,13 +5605,13 @@
         <v>37</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
@@ -5634,13 +5638,13 @@
         <v>37</v>
       </c>
       <c r="X36" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="Y36" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="Z36" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="AA36" t="s" s="2">
         <v>37</v>
@@ -5658,28 +5662,28 @@
         <v>37</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH36" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI36" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="AL36" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="AN36" t="s" s="2">
         <v>37</v>
@@ -5687,10 +5691,10 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -5713,16 +5717,16 @@
         <v>37</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="N37" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="O37" s="2"/>
       <c r="P37" t="s" s="2">
@@ -5748,13 +5752,13 @@
         <v>37</v>
       </c>
       <c r="X37" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="Y37" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="Z37" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="AA37" t="s" s="2">
         <v>37</v>
@@ -5772,28 +5776,28 @@
         <v>37</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH37" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI37" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="AL37" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>37</v>
@@ -5801,10 +5805,10 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
@@ -5824,22 +5828,22 @@
         <v>37</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="N38" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="O38" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="P38" t="s" s="2">
         <v>37</v>
@@ -5864,13 +5868,13 @@
         <v>37</v>
       </c>
       <c r="X38" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="Y38" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="Z38" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="AA38" t="s" s="2">
         <v>37</v>
@@ -5888,19 +5892,19 @@
         <v>37</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH38" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI38" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK38" t="s" s="2">
         <v>37</v>
@@ -5909,7 +5913,7 @@
         <v>37</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>37</v>
@@ -5917,10 +5921,10 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
@@ -5943,13 +5947,13 @@
         <v>37</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
@@ -6000,7 +6004,7 @@
         <v>37</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>38</v>
@@ -6012,10 +6016,10 @@
         <v>37</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="AL39" t="s" s="2">
         <v>37</v>
@@ -6029,10 +6033,10 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -6043,7 +6047,7 @@
         <v>38</v>
       </c>
       <c r="G40" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H40" t="s" s="2">
         <v>37</v>
@@ -6055,13 +6059,13 @@
         <v>37</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
@@ -6112,13 +6116,13 @@
         <v>37</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH40" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI40" t="s" s="2">
         <v>37</v>
@@ -6127,7 +6131,7 @@
         <v>37</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AL40" t="s" s="2">
         <v>37</v>
@@ -6141,14 +6145,14 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" t="s" s="2">
@@ -6167,16 +6171,16 @@
         <v>37</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="N41" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O41" s="2"/>
       <c r="P41" t="s" s="2">
@@ -6226,7 +6230,7 @@
         <v>37</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>38</v>
@@ -6238,10 +6242,10 @@
         <v>37</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AL41" t="s" s="2">
         <v>37</v>
@@ -6255,14 +6259,14 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" t="s" s="2">
@@ -6275,25 +6279,25 @@
         <v>37</v>
       </c>
       <c r="I42" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="N42" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O42" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="P42" t="s" s="2">
         <v>37</v>
@@ -6342,7 +6346,7 @@
         <v>37</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>38</v>
@@ -6354,10 +6358,10 @@
         <v>37</v>
       </c>
       <c r="AJ42" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AL42" t="s" s="2">
         <v>37</v>
@@ -6371,10 +6375,10 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -6385,7 +6389,7 @@
         <v>38</v>
       </c>
       <c r="G43" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H43" t="s" s="2">
         <v>37</v>
@@ -6397,13 +6401,13 @@
         <v>37</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" s="2"/>
@@ -6454,22 +6458,22 @@
         <v>37</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH43" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI43" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ43" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="AL43" t="s" s="2">
         <v>37</v>
@@ -6483,10 +6487,10 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -6497,7 +6501,7 @@
         <v>38</v>
       </c>
       <c r="G44" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H44" t="s" s="2">
         <v>37</v>
@@ -6509,13 +6513,13 @@
         <v>37</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
@@ -6542,13 +6546,13 @@
         <v>37</v>
       </c>
       <c r="X44" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="Y44" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="Z44" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="AA44" t="s" s="2">
         <v>37</v>
@@ -6566,22 +6570,22 @@
         <v>37</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH44" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI44" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ44" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="AL44" t="s" s="2">
         <v>37</v>
@@ -6595,10 +6599,10 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -6621,13 +6625,13 @@
         <v>37</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="N45" s="2"/>
       <c r="O45" s="2"/>
@@ -6678,7 +6682,7 @@
         <v>37</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>38</v>
@@ -6690,16 +6694,16 @@
         <v>37</v>
       </c>
       <c r="AJ45" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK45" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AL45" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="AN45" t="s" s="2">
         <v>37</v>
@@ -6707,10 +6711,10 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
@@ -6721,7 +6725,7 @@
         <v>38</v>
       </c>
       <c r="G46" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H46" t="s" s="2">
         <v>37</v>
@@ -6733,13 +6737,13 @@
         <v>37</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
@@ -6790,22 +6794,22 @@
         <v>37</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH46" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI46" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ46" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK46" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="AL46" t="s" s="2">
         <v>37</v>
@@ -6819,10 +6823,10 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
@@ -6845,13 +6849,13 @@
         <v>37</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="N47" s="2"/>
       <c r="O47" s="2"/>
@@ -6902,7 +6906,7 @@
         <v>37</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>38</v>
@@ -6914,10 +6918,10 @@
         <v>37</v>
       </c>
       <c r="AJ47" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="AL47" t="s" s="2">
         <v>37</v>
@@ -6931,10 +6935,10 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -6945,7 +6949,7 @@
         <v>38</v>
       </c>
       <c r="G48" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H48" t="s" s="2">
         <v>37</v>
@@ -6957,13 +6961,13 @@
         <v>37</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="N48" s="2"/>
       <c r="O48" s="2"/>
@@ -7014,13 +7018,13 @@
         <v>37</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH48" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI48" t="s" s="2">
         <v>37</v>
@@ -7029,7 +7033,7 @@
         <v>37</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AL48" t="s" s="2">
         <v>37</v>
@@ -7043,14 +7047,14 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" t="s" s="2">
@@ -7069,16 +7073,16 @@
         <v>37</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="N49" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O49" s="2"/>
       <c r="P49" t="s" s="2">
@@ -7128,7 +7132,7 @@
         <v>37</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>38</v>
@@ -7140,10 +7144,10 @@
         <v>37</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AL49" t="s" s="2">
         <v>37</v>
@@ -7157,14 +7161,14 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" t="s" s="2">
@@ -7177,25 +7181,25 @@
         <v>37</v>
       </c>
       <c r="I50" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="N50" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O50" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="P50" t="s" s="2">
         <v>37</v>
@@ -7244,7 +7248,7 @@
         <v>37</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>38</v>
@@ -7256,10 +7260,10 @@
         <v>37</v>
       </c>
       <c r="AJ50" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AL50" t="s" s="2">
         <v>37</v>
@@ -7273,10 +7277,10 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
@@ -7296,16 +7300,16 @@
         <v>37</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
@@ -7356,7 +7360,7 @@
         <v>37</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>38</v>
@@ -7368,16 +7372,16 @@
         <v>37</v>
       </c>
       <c r="AJ51" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="AL51" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>37</v>
@@ -7385,10 +7389,10 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
@@ -7399,7 +7403,7 @@
         <v>38</v>
       </c>
       <c r="G52" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H52" t="s" s="2">
         <v>37</v>
@@ -7411,13 +7415,13 @@
         <v>37</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="N52" s="2"/>
       <c r="O52" s="2"/>
@@ -7468,22 +7472,22 @@
         <v>37</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH52" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI52" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ52" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="AL52" t="s" s="2">
         <v>37</v>
@@ -7497,10 +7501,10 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
@@ -7511,7 +7515,7 @@
         <v>38</v>
       </c>
       <c r="G53" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H53" t="s" s="2">
         <v>37</v>
@@ -7523,13 +7527,13 @@
         <v>37</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="N53" s="2"/>
       <c r="O53" s="2"/>
@@ -7556,13 +7560,13 @@
         <v>37</v>
       </c>
       <c r="X53" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="Y53" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="Z53" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="AA53" t="s" s="2">
         <v>37</v>
@@ -7580,28 +7584,28 @@
         <v>37</v>
       </c>
       <c r="AF53" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="AG53" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH53" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI53" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ53" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="AL53" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="AN53" t="s" s="2">
         <v>37</v>
@@ -7609,10 +7613,10 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" t="s" s="2">
@@ -7623,7 +7627,7 @@
         <v>38</v>
       </c>
       <c r="G54" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H54" t="s" s="2">
         <v>37</v>
@@ -7635,13 +7639,13 @@
         <v>37</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="N54" s="2"/>
       <c r="O54" s="2"/>
@@ -7692,28 +7696,28 @@
         <v>37</v>
       </c>
       <c r="AF54" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="AG54" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH54" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI54" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ54" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK54" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="AL54" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="AN54" t="s" s="2">
         <v>37</v>
@@ -7721,10 +7725,10 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" t="s" s="2">
@@ -7735,7 +7739,7 @@
         <v>38</v>
       </c>
       <c r="G55" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H55" t="s" s="2">
         <v>37</v>
@@ -7747,13 +7751,13 @@
         <v>37</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="N55" s="2"/>
       <c r="O55" s="2"/>
@@ -7804,28 +7808,28 @@
         <v>37</v>
       </c>
       <c r="AF55" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="AG55" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH55" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI55" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ55" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK55" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="AL55" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM55" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="AN55" t="s" s="2">
         <v>37</v>
@@ -7833,10 +7837,10 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" t="s" s="2">
@@ -7847,7 +7851,7 @@
         <v>38</v>
       </c>
       <c r="G56" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H56" t="s" s="2">
         <v>37</v>
@@ -7859,13 +7863,13 @@
         <v>37</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="N56" s="2"/>
       <c r="O56" s="2"/>
@@ -7892,13 +7896,13 @@
         <v>37</v>
       </c>
       <c r="X56" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="Y56" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="Z56" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="AA56" t="s" s="2">
         <v>37</v>
@@ -7916,28 +7920,28 @@
         <v>37</v>
       </c>
       <c r="AF56" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="AG56" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AH56" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI56" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AJ56" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="AL56" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM56" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="AN56" t="s" s="2">
         <v>37</v>
@@ -7945,10 +7949,10 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" t="s" s="2">
@@ -7968,22 +7972,22 @@
         <v>37</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="N57" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="O57" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="P57" t="s" s="2">
         <v>37</v>
@@ -8008,13 +8012,13 @@
         <v>37</v>
       </c>
       <c r="X57" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="Y57" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="Z57" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="AA57" t="s" s="2">
         <v>37</v>
@@ -8032,7 +8036,7 @@
         <v>37</v>
       </c>
       <c r="AF57" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="AG57" t="s" s="2">
         <v>38</v>
@@ -8044,7 +8048,7 @@
         <v>37</v>
       </c>
       <c r="AJ57" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK57" t="s" s="2">
         <v>37</v>
@@ -8053,7 +8057,7 @@
         <v>37</v>
       </c>
       <c r="AM57" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="AN57" t="s" s="2">
         <v>37</v>
@@ -8061,10 +8065,10 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" t="s" s="2">
@@ -8087,13 +8091,13 @@
         <v>37</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="N58" s="2"/>
       <c r="O58" s="2"/>
@@ -8144,7 +8148,7 @@
         <v>37</v>
       </c>
       <c r="AF58" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="AG58" t="s" s="2">
         <v>38</v>
@@ -8156,16 +8160,16 @@
         <v>37</v>
       </c>
       <c r="AJ58" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="AL58" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM58" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="AN58" t="s" s="2">
         <v>37</v>

</xml_diff>